<commit_message>
Fix typo in column name
</commit_message>
<xml_diff>
--- a/data/covid19_MTL.xlsx
+++ b/data/covid19_MTL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D433E668-0F1E-4FFC-A173-1C5A231624CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C607EE-C432-484A-A609-C35B68C4585D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25000" yWindow="8040" windowWidth="12710" windowHeight="9740" tabRatio="765" activeTab="2" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -748,9 +748,6 @@
     <t>6 AVRIL, 16H 55</t>
   </si>
   <si>
-    <t>deaths_tml</t>
-  </si>
-  <si>
     <t>Deaths</t>
   </si>
   <si>
@@ -854,6 +851,9 @@
   </si>
   <si>
     <t>639,3</t>
+  </si>
+  <si>
+    <t>deaths_mtl</t>
   </si>
 </sst>
 </file>
@@ -4118,14 +4118,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9609F4-1A5A-459D-8297-63DB4B7007A3}">
   <dimension ref="A1:AR25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AR25" sqref="AR25"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.6328125" customWidth="1"/>
-    <col min="2" max="14" width="8.6328125" customWidth="1"/>
+    <col min="2" max="3" width="8.6328125" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" customWidth="1"/>
+    <col min="5" max="14" width="8.6328125" customWidth="1"/>
     <col min="15" max="15" width="12.81640625" customWidth="1"/>
     <col min="16" max="16" width="8.6328125" customWidth="1"/>
   </cols>
@@ -4141,7 +4143,7 @@
         <v>182</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>145</v>
@@ -8975,7 +8977,7 @@
         <v>2837</v>
       </c>
       <c r="G21">
-        <f>C21-F21</f>
+        <f t="shared" ref="G21:G26" si="2">C21-F21</f>
         <v>408</v>
       </c>
     </row>
@@ -8997,7 +8999,7 @@
         <v>3261</v>
       </c>
       <c r="G22">
-        <f>C22-F22</f>
+        <f t="shared" si="2"/>
         <v>348</v>
       </c>
     </row>
@@ -9019,7 +9021,7 @@
         <v>3713</v>
       </c>
       <c r="G23">
-        <f>C23-F23</f>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
     </row>
@@ -9041,7 +9043,7 @@
         <v>3977</v>
       </c>
       <c r="G24">
-        <f>C24-F24</f>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
     </row>
@@ -9063,7 +9065,7 @@
         <v>4407</v>
       </c>
       <c r="G25">
-        <f>C25-F25</f>
+        <f t="shared" si="2"/>
         <v>218</v>
       </c>
     </row>
@@ -9085,7 +9087,7 @@
         <v>4408</v>
       </c>
       <c r="G26">
-        <f>C26-F26</f>
+        <f t="shared" si="2"/>
         <v>367</v>
       </c>
     </row>
@@ -9140,7 +9142,7 @@
         <v>223</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -10509,7 +10511,7 @@
         <v>223</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -10812,7 +10814,7 @@
         <v>223</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
@@ -10845,10 +10847,10 @@
         <v>215</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
@@ -10881,10 +10883,10 @@
         <v>216</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
@@ -10917,10 +10919,10 @@
         <v>217</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
@@ -10953,10 +10955,10 @@
         <v>218</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -10989,10 +10991,10 @@
         <v>219</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
@@ -11083,7 +11085,7 @@
         <v>223</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
@@ -11526,7 +11528,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B70" t="s">
         <v>102</v>
@@ -11583,10 +11585,10 @@
         <v>86</v>
       </c>
       <c r="B1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" t="s">
         <v>232</v>
-      </c>
-      <c r="C1" t="s">
-        <v>233</v>
       </c>
       <c r="D1" t="s">
         <v>183</v>
@@ -11610,10 +11612,10 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="s">
         <v>243</v>
-      </c>
-      <c r="D4" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -11627,7 +11629,7 @@
         <v>221</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -11641,7 +11643,7 @@
         <v>220</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -11652,10 +11654,10 @@
         <v>696</v>
       </c>
       <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" t="s">
         <v>247</v>
-      </c>
-      <c r="D7" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -11666,10 +11668,10 @@
         <v>772</v>
       </c>
       <c r="C8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -11680,10 +11682,10 @@
         <v>837</v>
       </c>
       <c r="C9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" t="s">
         <v>250</v>
-      </c>
-      <c r="D9" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -11694,10 +11696,10 @@
         <v>708</v>
       </c>
       <c r="C10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" t="s">
         <v>252</v>
-      </c>
-      <c r="D10" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -11708,10 +11710,10 @@
         <v>505</v>
       </c>
       <c r="C11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" t="s">
         <v>254</v>
-      </c>
-      <c r="D11" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -11722,10 +11724,10 @@
         <v>368</v>
       </c>
       <c r="C12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" t="s">
         <v>256</v>
-      </c>
-      <c r="D12" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -11736,10 +11738,10 @@
         <v>646</v>
       </c>
       <c r="C13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" t="s">
         <v>258</v>
-      </c>
-      <c r="D13" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -11750,10 +11752,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -11761,13 +11763,13 @@
         <v>98</v>
       </c>
       <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" t="s">
         <v>240</v>
-      </c>
-      <c r="C15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D15" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update data (2020-04-10 v2)
Santé Montréal posted additional data.
</commit_message>
<xml_diff>
--- a/data/covid19_MTL.xlsx
+++ b/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B3198A-B705-48CB-B514-83D5950A40A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2127EC4-C5C9-42B8-8334-9DD16B58B36B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10130" yWindow="3190" windowWidth="28170" windowHeight="17470" tabRatio="765" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="9200" yWindow="3520" windowWidth="28170" windowHeight="17470" tabRatio="765" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="327">
   <si>
     <t>borough</t>
   </si>
@@ -790,9 +790,6 @@
     <t>deaths_mtl</t>
   </si>
   <si>
-    <t>5 262</t>
-  </si>
-  <si>
     <t>8 AVRIL, 17H</t>
   </si>
   <si>
@@ -814,37 +811,250 @@
     <t>254,7 </t>
   </si>
   <si>
-    <t>TOTAL DE DÉCÈS</t>
-  </si>
-  <si>
-    <t>1 178</t>
-  </si>
-  <si>
-    <t>27,0</t>
-  </si>
-  <si>
     <t>317,0</t>
   </si>
   <si>
-    <t>16,9</t>
-  </si>
-  <si>
     <t>229,8</t>
   </si>
   <si>
-    <t>19,4 </t>
-  </si>
-  <si>
-    <t>15,7 </t>
-  </si>
-  <si>
     <t>Territoire à confirmer²</t>
   </si>
   <si>
-    <t>1 190</t>
-  </si>
-  <si>
     <t>9 AVRIL, 17H</t>
+  </si>
+  <si>
+    <t>193,7</t>
+  </si>
+  <si>
+    <t>175,3</t>
+  </si>
+  <si>
+    <t>5 617</t>
+  </si>
+  <si>
+    <t>271,9 </t>
+  </si>
+  <si>
+    <t>271,9</t>
+  </si>
+  <si>
+    <t>ARRONDISSEMENT OU VILLE LIÉE</t>
+  </si>
+  <si>
+    <t>6,3</t>
+  </si>
+  <si>
+    <t>206,3</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>156,6</t>
+  </si>
+  <si>
+    <t>Baie-D'Urfé    </t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t> n.p.</t>
+  </si>
+  <si>
+    <t>Beaconsfield    </t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>* 72,4</t>
+  </si>
+  <si>
+    <t>11,9</t>
+  </si>
+  <si>
+    <t>313,5</t>
+  </si>
+  <si>
+    <t>Côte-Saint-Luc    </t>
+  </si>
+  <si>
+    <t>6,0</t>
+  </si>
+  <si>
+    <t>813,6</t>
+  </si>
+  <si>
+    <t>Dollard-des-Ormeaux    </t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>139,1</t>
+  </si>
+  <si>
+    <t>Dorval  </t>
+  </si>
+  <si>
+    <t>0,8</t>
+  </si>
+  <si>
+    <t>194,9</t>
+  </si>
+  <si>
+    <t>Hampstead    </t>
+  </si>
+  <si>
+    <t> 0,7</t>
+  </si>
+  <si>
+    <t>* 415,9</t>
+  </si>
+  <si>
+    <t>Kirkland    </t>
+  </si>
+  <si>
+    <t>* 74,4</t>
+  </si>
+  <si>
+    <t>2,0 </t>
+  </si>
+  <si>
+    <t>186,6</t>
+  </si>
+  <si>
+    <t>6,8</t>
+  </si>
+  <si>
+    <t>387,8</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>* 119,5</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>170,6</t>
+  </si>
+  <si>
+    <t>Montréal-Est    </t>
+  </si>
+  <si>
+    <t>0,2 </t>
+  </si>
+  <si>
+    <t>n.p.</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>282,5</t>
+  </si>
+  <si>
+    <t>Montréal-Ouest    </t>
+  </si>
+  <si>
+    <t>Mont-Royal    </t>
+  </si>
+  <si>
+    <t>1,1  </t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>1,8</t>
+  </si>
+  <si>
+    <t>112,6</t>
+  </si>
+  <si>
+    <t>223,1</t>
+  </si>
+  <si>
+    <t>Pointe-Claire    </t>
+  </si>
+  <si>
+    <t>0,8 </t>
+  </si>
+  <si>
+    <t>* 105,2</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>181,7</t>
+  </si>
+  <si>
+    <t>5,9</t>
+  </si>
+  <si>
+    <t>186,3</t>
+  </si>
+  <si>
+    <t>Sainte-Anne-de-Bellevue    </t>
+  </si>
+  <si>
+    <t>3,8</t>
+  </si>
+  <si>
+    <t>169,0</t>
+  </si>
+  <si>
+    <t>3,2 </t>
+  </si>
+  <si>
+    <t>177,5</t>
+  </si>
+  <si>
+    <t>Senneville    </t>
+  </si>
+  <si>
+    <t>4,8</t>
+  </si>
+  <si>
+    <t>268,7</t>
+  </si>
+  <si>
+    <t>4,0</t>
+  </si>
+  <si>
+    <t>251,3</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>207,5</t>
+  </si>
+  <si>
+    <t>6,1</t>
+  </si>
+  <si>
+    <t>184,9</t>
+  </si>
+  <si>
+    <t>Westmount    </t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>280,6</t>
+  </si>
+  <si>
+    <t>1 245</t>
+  </si>
+  <si>
+    <t>Total à Montréal    </t>
   </si>
 </sst>
 </file>
@@ -1437,8 +1647,8 @@
       <c r="L2">
         <v>247</v>
       </c>
-      <c r="M2" t="s">
-        <v>102</v>
+      <c r="M2">
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1478,8 +1688,8 @@
       <c r="L3">
         <v>59</v>
       </c>
-      <c r="M3" t="s">
-        <v>102</v>
+      <c r="M3">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -1519,8 +1729,8 @@
       <c r="L4">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
-        <v>102</v>
+      <c r="M4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -1560,8 +1770,8 @@
       <c r="L5">
         <v>14</v>
       </c>
-      <c r="M5" t="s">
-        <v>102</v>
+      <c r="M5">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -1601,8 +1811,8 @@
       <c r="L6">
         <v>501</v>
       </c>
-      <c r="M6" t="s">
-        <v>102</v>
+      <c r="M6">
+        <v>522</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -1642,8 +1852,8 @@
       <c r="L7">
         <v>262</v>
       </c>
-      <c r="M7" t="s">
-        <v>102</v>
+      <c r="M7">
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -1683,8 +1893,8 @@
       <c r="L8">
         <v>66</v>
       </c>
-      <c r="M8" t="s">
-        <v>102</v>
+      <c r="M8">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -1724,8 +1934,8 @@
       <c r="L9">
         <v>37</v>
       </c>
-      <c r="M9" t="s">
-        <v>102</v>
+      <c r="M9">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -1765,8 +1975,8 @@
       <c r="L10">
         <v>29</v>
       </c>
-      <c r="M10" t="s">
-        <v>102</v>
+      <c r="M10">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -1806,8 +2016,8 @@
       <c r="L11">
         <v>14</v>
       </c>
-      <c r="M11" t="s">
-        <v>102</v>
+      <c r="M11">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -1847,8 +2057,8 @@
       <c r="L12">
         <v>83</v>
       </c>
-      <c r="M12" t="s">
-        <v>102</v>
+      <c r="M12">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -1888,8 +2098,8 @@
       <c r="L13">
         <v>286</v>
       </c>
-      <c r="M13" t="s">
-        <v>102</v>
+      <c r="M13">
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -1929,8 +2139,8 @@
       <c r="L14">
         <v>19</v>
       </c>
-      <c r="M14" t="s">
-        <v>102</v>
+      <c r="M14">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -1970,8 +2180,8 @@
       <c r="L15">
         <v>213</v>
       </c>
-      <c r="M15" t="s">
-        <v>102</v>
+      <c r="M15">
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -2011,8 +2221,8 @@
       <c r="L16">
         <v>6</v>
       </c>
-      <c r="M16" t="s">
-        <v>102</v>
+      <c r="M16">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
@@ -2052,8 +2262,8 @@
       <c r="L17">
         <v>193</v>
       </c>
-      <c r="M17" t="s">
-        <v>102</v>
+      <c r="M17">
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -2093,8 +2303,8 @@
       <c r="L18">
         <v>5</v>
       </c>
-      <c r="M18" t="s">
-        <v>102</v>
+      <c r="M18">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -2134,8 +2344,8 @@
       <c r="L19">
         <v>44</v>
       </c>
-      <c r="M19" t="s">
-        <v>102</v>
+      <c r="M19">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
@@ -2175,8 +2385,8 @@
       <c r="L20">
         <v>139</v>
       </c>
-      <c r="M20" t="s">
-        <v>102</v>
+      <c r="M20">
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -2216,8 +2426,8 @@
       <c r="L21">
         <v>75</v>
       </c>
-      <c r="M21" t="s">
-        <v>102</v>
+      <c r="M21">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
@@ -2257,8 +2467,8 @@
       <c r="L22">
         <v>220</v>
       </c>
-      <c r="M22" t="s">
-        <v>102</v>
+      <c r="M22">
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -2298,8 +2508,8 @@
       <c r="L23">
         <v>32</v>
       </c>
-      <c r="M23" t="s">
-        <v>102</v>
+      <c r="M23">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
@@ -2339,8 +2549,8 @@
       <c r="L24">
         <v>180</v>
       </c>
-      <c r="M24" t="s">
-        <v>102</v>
+      <c r="M24">
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -2380,8 +2590,8 @@
       <c r="L25">
         <v>247</v>
       </c>
-      <c r="M25" t="s">
-        <v>102</v>
+      <c r="M25">
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -2421,8 +2631,8 @@
       <c r="L26">
         <v>5</v>
       </c>
-      <c r="M26" t="s">
-        <v>102</v>
+      <c r="M26">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -2462,8 +2672,8 @@
       <c r="L27">
         <v>163</v>
       </c>
-      <c r="M27" t="s">
-        <v>102</v>
+      <c r="M27">
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
@@ -2503,8 +2713,8 @@
       <c r="L28">
         <v>124</v>
       </c>
-      <c r="M28" t="s">
-        <v>102</v>
+      <c r="M28">
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -2544,8 +2754,8 @@
       <c r="L29">
         <v>2</v>
       </c>
-      <c r="M29" t="s">
-        <v>102</v>
+      <c r="M29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -2585,8 +2795,8 @@
       <c r="L30">
         <v>184</v>
       </c>
-      <c r="M30" t="s">
-        <v>102</v>
+      <c r="M30">
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -2626,8 +2836,8 @@
       <c r="L31">
         <v>154</v>
       </c>
-      <c r="M31" t="s">
-        <v>102</v>
+      <c r="M31">
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -2667,8 +2877,8 @@
       <c r="L32">
         <v>174</v>
       </c>
-      <c r="M32" t="s">
-        <v>102</v>
+      <c r="M32">
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -2708,8 +2918,8 @@
       <c r="L33">
         <v>242</v>
       </c>
-      <c r="M33" t="s">
-        <v>102</v>
+      <c r="M33">
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -2749,8 +2959,8 @@
       <c r="L34">
         <v>57</v>
       </c>
-      <c r="M34" t="s">
-        <v>102</v>
+      <c r="M34">
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
@@ -2790,8 +3000,8 @@
       <c r="L35">
         <v>1181</v>
       </c>
-      <c r="M35" t="s">
-        <v>102</v>
+      <c r="M35">
+        <v>1245</v>
       </c>
     </row>
   </sheetData>
@@ -2804,7 +3014,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2913,8 +3123,9 @@
         <f>cases!L2/(population_2016!$B2/1000)</f>
         <v>1.8399195500763528</v>
       </c>
-      <c r="M2" t="s">
-        <v>102</v>
+      <c r="M2" s="3">
+        <f>cases!M2/(population_2016!$B2/1000)</f>
+        <v>2.063391560207084</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -2964,8 +3175,9 @@
         <f>cases!L3/(population_2016!$B3/1000)</f>
         <v>1.3786335171511357</v>
       </c>
-      <c r="M3" t="s">
-        <v>102</v>
+      <c r="M3" s="3">
+        <f>cases!M3/(population_2016!$B3/1000)</f>
+        <v>1.5655668754089167</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -3015,8 +3227,9 @@
         <f>cases!L4/(population_2016!$B4/1000)</f>
         <v>1.3078733978550876</v>
       </c>
-      <c r="M4" t="s">
-        <v>102</v>
+      <c r="M4" s="3">
+        <f>cases!M4/(population_2016!$B4/1000)</f>
+        <v>1.3078733978550876</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -3066,8 +3279,9 @@
         <f>cases!L5/(population_2016!$B5/1000)</f>
         <v>0.72448768370937688</v>
       </c>
-      <c r="M5" t="s">
-        <v>102</v>
+      <c r="M5" s="3">
+        <f>cases!M5/(population_2016!$B5/1000)</f>
+        <v>0.72448768370937688</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -3117,8 +3331,9 @@
         <f>cases!L6/(population_2016!$B6/1000)</f>
         <v>3.008647609896709</v>
       </c>
-      <c r="M6" t="s">
-        <v>102</v>
+      <c r="M6" s="3">
+        <f>cases!M6/(population_2016!$B6/1000)</f>
+        <v>3.1347585875570498</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -3168,8 +3383,9 @@
         <f>cases!L7/(population_2016!$B7/1000)</f>
         <v>8.0744575936883631</v>
       </c>
-      <c r="M7" t="s">
-        <v>102</v>
+      <c r="M7" s="3">
+        <f>cases!M7/(population_2016!$B7/1000)</f>
+        <v>8.1360946745562135</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -3219,8 +3435,9 @@
         <f>cases!L8/(population_2016!$B8/1000)</f>
         <v>1.3497208531871818</v>
       </c>
-      <c r="M8" t="s">
-        <v>102</v>
+      <c r="M8" s="3">
+        <f>cases!M8/(population_2016!$B8/1000)</f>
+        <v>1.3906214851019447</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -3270,8 +3487,9 @@
         <f>cases!L9/(population_2016!$B9/1000)</f>
         <v>1.9494204425711275</v>
       </c>
-      <c r="M9" t="s">
-        <v>102</v>
+      <c r="M9" s="3">
+        <f>cases!M9/(population_2016!$B9/1000)</f>
+        <v>1.9494204425711275</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -3321,8 +3539,9 @@
         <f>cases!L10/(population_2016!$B10/1000)</f>
         <v>4.1588986089201203</v>
       </c>
-      <c r="M10" t="s">
-        <v>102</v>
+      <c r="M10" s="3">
+        <f>cases!M10/(population_2016!$B10/1000)</f>
+        <v>4.1588986089201203</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -3372,8 +3591,9 @@
         <f>cases!L11/(population_2016!$B11/1000)</f>
         <v>0.69475460274924317</v>
       </c>
-      <c r="M11" t="s">
-        <v>102</v>
+      <c r="M11" s="3">
+        <f>cases!M11/(population_2016!$B11/1000)</f>
+        <v>0.74437993151704629</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -3423,8 +3643,9 @@
         <f>cases!L12/(population_2016!$B12/1000)</f>
         <v>1.8656297062195151</v>
       </c>
-      <c r="M12" t="s">
-        <v>102</v>
+      <c r="M12" s="3">
+        <f>cases!M12/(population_2016!$B12/1000)</f>
+        <v>1.8656297062195151</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -3474,8 +3695,9 @@
         <f>cases!L13/(population_2016!$B13/1000)</f>
         <v>3.7213901864598653</v>
       </c>
-      <c r="M13" t="s">
-        <v>102</v>
+      <c r="M13" s="3">
+        <f>cases!M13/(population_2016!$B13/1000)</f>
+        <v>3.8775324320455939</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -3525,8 +3747,9 @@
         <f>cases!L14/(population_2016!$B14/1000)</f>
         <v>1.0318796502471079</v>
       </c>
-      <c r="M14" t="s">
-        <v>102</v>
+      <c r="M14" s="3">
+        <f>cases!M14/(population_2016!$B14/1000)</f>
+        <v>1.1948080160755987</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -3576,8 +3799,9 @@
         <f>cases!L15/(population_2016!$B15/1000)</f>
         <v>1.5659001352702464</v>
       </c>
-      <c r="M15" t="s">
-        <v>102</v>
+      <c r="M15" s="3">
+        <f>cases!M15/(population_2016!$B15/1000)</f>
+        <v>1.7055813679938834</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -3627,8 +3851,9 @@
         <f>cases!L16/(population_2016!$B16/1000)</f>
         <v>1.5584415584415585</v>
       </c>
-      <c r="M16" t="s">
-        <v>102</v>
+      <c r="M16" s="3">
+        <f>cases!M16/(population_2016!$B16/1000)</f>
+        <v>1.8181818181818181</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
@@ -3678,8 +3903,9 @@
         <f>cases!L17/(population_2016!$B17/1000)</f>
         <v>2.2912363178763919</v>
       </c>
-      <c r="M17" t="s">
-        <v>102</v>
+      <c r="M17" s="3">
+        <f>cases!M17/(population_2016!$B17/1000)</f>
+        <v>2.8254624023553436</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -3729,8 +3955,9 @@
         <f>cases!L18/(population_2016!$B18/1000)</f>
         <v>0.99009900990099009</v>
       </c>
-      <c r="M18" t="s">
-        <v>102</v>
+      <c r="M18" s="3">
+        <f>cases!M18/(population_2016!$B18/1000)</f>
+        <v>0.99009900990099009</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -3780,8 +4007,9 @@
         <f>cases!L19/(population_2016!$B19/1000)</f>
         <v>2.170053264943776</v>
       </c>
-      <c r="M19" t="s">
-        <v>102</v>
+      <c r="M19" s="3">
+        <f>cases!M19/(population_2016!$B19/1000)</f>
+        <v>2.170053264943776</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
@@ -3831,8 +4059,9 @@
         <f>cases!L20/(population_2016!$B20/1000)</f>
         <v>5.8027886783000753</v>
       </c>
-      <c r="M20" t="s">
-        <v>102</v>
+      <c r="M20" s="3">
+        <f>cases!M20/(population_2016!$B20/1000)</f>
+        <v>5.9697754028554728</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -3882,8 +4111,9 @@
         <f>cases!L21/(population_2016!$B21/1000)</f>
         <v>1.0822979349755402</v>
       </c>
-      <c r="M21" t="s">
-        <v>102</v>
+      <c r="M21" s="3">
+        <f>cases!M21/(population_2016!$B21/1000)</f>
+        <v>1.1255898523745618</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
@@ -3933,8 +4163,9 @@
         <f>cases!L22/(population_2016!$B22/1000)</f>
         <v>2.1153846153846154</v>
       </c>
-      <c r="M22" t="s">
-        <v>102</v>
+      <c r="M22" s="3">
+        <f>cases!M22/(population_2016!$B22/1000)</f>
+        <v>2.2307692307692308</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -3984,8 +4215,9 @@
         <f>cases!L23/(population_2016!$B23/1000)</f>
         <v>1.0197578075207139</v>
       </c>
-      <c r="M23" t="s">
-        <v>102</v>
+      <c r="M23" s="3">
+        <f>cases!M23/(population_2016!$B23/1000)</f>
+        <v>1.0516252390057361</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
@@ -4035,8 +4267,9 @@
         <f>cases!L24/(population_2016!$B24/1000)</f>
         <v>1.6862932463955482</v>
       </c>
-      <c r="M24" t="s">
-        <v>102</v>
+      <c r="M24" s="3">
+        <f>cases!M24/(population_2016!$B24/1000)</f>
+        <v>1.8174493877818687</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -4086,8 +4319,9 @@
         <f>cases!L25/(population_2016!$B25/1000)</f>
         <v>1.7694677269145354</v>
       </c>
-      <c r="M25" t="s">
-        <v>102</v>
+      <c r="M25" s="3">
+        <f>cases!M25/(population_2016!$B25/1000)</f>
+        <v>1.8625976072784582</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -4137,8 +4371,9 @@
         <f>cases!L26/(population_2016!$B26/1000)</f>
         <v>1.008471157724889</v>
       </c>
-      <c r="M26" t="s">
-        <v>102</v>
+      <c r="M26" s="3">
+        <f>cases!M26/(population_2016!$B26/1000)</f>
+        <v>1.008471157724889</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -4188,8 +4423,9 @@
         <f>cases!L27/(population_2016!$B27/1000)</f>
         <v>1.6493301493503865</v>
       </c>
-      <c r="M27" t="s">
-        <v>102</v>
+      <c r="M27" s="3">
+        <f>cases!M27/(population_2016!$B27/1000)</f>
+        <v>1.6898045088436475</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
@@ -4239,8 +4475,9 @@
         <f>cases!L28/(population_2016!$B28/1000)</f>
         <v>1.5835514973501053</v>
       </c>
-      <c r="M28" t="s">
-        <v>102</v>
+      <c r="M28" s="3">
+        <f>cases!M28/(population_2016!$B28/1000)</f>
+        <v>1.7751101462231018</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -4290,8 +4527,9 @@
         <f>cases!L29/(population_2016!$B29/1000)</f>
         <v>2.1715526601520088</v>
       </c>
-      <c r="M29" t="s">
-        <v>102</v>
+      <c r="M29" s="3">
+        <f>cases!M29/(population_2016!$B29/1000)</f>
+        <v>2.1715526601520088</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -4341,8 +4579,9 @@
         <f>cases!L30/(population_2016!$B30/1000)</f>
         <v>2.3544164502053717</v>
       </c>
-      <c r="M30" t="s">
-        <v>102</v>
+      <c r="M30" s="3">
+        <f>cases!M30/(population_2016!$B30/1000)</f>
+        <v>2.6871057312126525</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -4392,8 +4631,9 @@
         <f>cases!L31/(population_2016!$B31/1000)</f>
         <v>2.2245012928108161</v>
       </c>
-      <c r="M31" t="s">
-        <v>102</v>
+      <c r="M31" s="3">
+        <f>cases!M31/(population_2016!$B31/1000)</f>
+        <v>2.5133975646044289</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -4443,8 +4683,9 @@
         <f>cases!L32/(population_2016!$B32/1000)</f>
         <v>1.951328922283279</v>
       </c>
-      <c r="M32" t="s">
-        <v>102</v>
+      <c r="M32" s="3">
+        <f>cases!M32/(population_2016!$B32/1000)</f>
+        <v>2.0746887966804981</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -4494,8 +4735,9 @@
         <f>cases!L33/(population_2016!$B33/1000)</f>
         <v>1.6822728757829173</v>
       </c>
-      <c r="M33" t="s">
-        <v>102</v>
+      <c r="M33" s="3">
+        <f>cases!M33/(population_2016!$B33/1000)</f>
+        <v>1.8491098551994047</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -4545,8 +4787,9 @@
         <f>cases!L34/(population_2016!$B34/1000)</f>
         <v>2.8062229224103978</v>
       </c>
-      <c r="M34" t="s">
-        <v>102</v>
+      <c r="M34" s="3">
+        <f>cases!M34/(population_2016!$B34/1000)</f>
+        <v>2.8062229224103978</v>
       </c>
     </row>
   </sheetData>
@@ -4559,7 +4802,7 @@
   <dimension ref="A1:AR27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+      <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6888,11 +7131,11 @@
       </c>
       <c r="B18" s="17">
         <f>mtl_newcases!C19</f>
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="C18" s="17">
         <f>mtl_newcases!B19</f>
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>102</v>
@@ -7055,7 +7298,7 @@
       </c>
       <c r="B19" s="17">
         <f>mtl_newcases!C20</f>
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="C19" s="17">
         <f>mtl_newcases!B20</f>
@@ -7222,7 +7465,7 @@
       </c>
       <c r="B20" s="17">
         <f>mtl_newcases!C21</f>
-        <v>3244</v>
+        <v>3243</v>
       </c>
       <c r="C20" s="17">
         <f>mtl_newcases!B21</f>
@@ -7389,7 +7632,7 @@
       </c>
       <c r="B21" s="17">
         <f>mtl_newcases!C22</f>
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="C21" s="17">
         <f>mtl_newcases!B22</f>
@@ -7556,7 +7799,7 @@
       </c>
       <c r="B22" s="17">
         <f>mtl_newcases!C23</f>
-        <v>3932</v>
+        <v>3931</v>
       </c>
       <c r="C22" s="17">
         <f>mtl_newcases!B23</f>
@@ -7713,7 +7956,7 @@
         <v>11.98022464872172</v>
       </c>
       <c r="AR22" s="3">
-        <f>X22*100/SUM($O22:$X22)</f>
+        <f t="shared" ref="AR22:AR27" si="22">X22*100/SUM($O22:$X22)</f>
         <v>20.492100354218103</v>
       </c>
     </row>
@@ -7723,7 +7966,7 @@
       </c>
       <c r="B23" s="17">
         <f>mtl_newcases!C24</f>
-        <v>4196</v>
+        <v>4195</v>
       </c>
       <c r="C23" s="17">
         <f>mtl_newcases!B24</f>
@@ -7804,83 +8047,83 @@
         <v>448.35787662567685</v>
       </c>
       <c r="Y23" s="3">
-        <f t="shared" ref="Y23" si="22">E23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="Y23" si="23">E23*100/SUM($E23:$N23)</f>
         <v>0.68078668683812404</v>
       </c>
       <c r="Z23" s="3">
-        <f t="shared" ref="Z23" si="23">F23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="Z23" si="24">F23*100/SUM($E23:$N23)</f>
         <v>0.73121533030761476</v>
       </c>
       <c r="AA23" s="3">
-        <f t="shared" ref="AA23" si="24">G23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AA23" si="25">G23*100/SUM($E23:$N23)</f>
         <v>3.7317196167423097</v>
       </c>
       <c r="AB23" s="3">
-        <f t="shared" ref="AB23" si="25">H23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AB23" si="26">H23*100/SUM($E23:$N23)</f>
         <v>15.683308119011599</v>
       </c>
       <c r="AC23" s="3">
-        <f t="shared" ref="AC23" si="26">I23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AC23" si="27">I23*100/SUM($E23:$N23)</f>
         <v>16.817952597075138</v>
       </c>
       <c r="AD23" s="3">
-        <f t="shared" ref="AD23" si="27">J23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AD23" si="28">J23*100/SUM($E23:$N23)</f>
         <v>17.423096318709028</v>
       </c>
       <c r="AE23" s="3">
-        <f t="shared" ref="AE23" si="28">K23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AE23" si="29">K23*100/SUM($E23:$N23)</f>
         <v>15.305093292990419</v>
       </c>
       <c r="AF23" s="3">
-        <f t="shared" ref="AF23" si="29">L23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AF23" si="30">L23*100/SUM($E23:$N23)</f>
         <v>10.91780131114473</v>
       </c>
       <c r="AG23" s="3">
-        <f t="shared" ref="AG23" si="30">M23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AG23" si="31">M23*100/SUM($E23:$N23)</f>
         <v>7.5390821986888552</v>
       </c>
       <c r="AH23" s="3">
-        <f t="shared" ref="AH23" si="31">N23*100/SUM($E23:$N23)</f>
+        <f t="shared" ref="AH23" si="32">N23*100/SUM($E23:$N23)</f>
         <v>11.169944528492184</v>
       </c>
       <c r="AI23" s="3">
-        <f t="shared" ref="AI23" si="32">O23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AI23" si="33">O23*100/SUM($O23:$X23)</f>
         <v>0.54469563009709021</v>
       </c>
       <c r="AJ23" s="3">
-        <f t="shared" ref="AJ23" si="33">P23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AJ23" si="34">P23*100/SUM($O23:$X23)</f>
         <v>1.4262483412011995</v>
       </c>
       <c r="AK23" s="3">
-        <f t="shared" ref="AK23" si="34">Q23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AK23" si="35">Q23*100/SUM($O23:$X23)</f>
         <v>4.0374946697262333</v>
       </c>
       <c r="AL23" s="3">
-        <f t="shared" ref="AL23" si="35">R23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AL23" si="36">R23*100/SUM($O23:$X23)</f>
         <v>10.889918755562032</v>
       </c>
       <c r="AM23" s="3">
-        <f t="shared" ref="AM23" si="36">S23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AM23" si="37">S23*100/SUM($O23:$X23)</f>
         <v>11.426430170066256</v>
       </c>
       <c r="AN23" s="3">
-        <f t="shared" ref="AN23" si="37">T23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AN23" si="38">T23*100/SUM($O23:$X23)</f>
         <v>13.940173348040345</v>
       </c>
       <c r="AO23" s="3">
-        <f t="shared" ref="AO23" si="38">U23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AO23" si="39">U23*100/SUM($O23:$X23)</f>
         <v>12.037431510940417</v>
       </c>
       <c r="AP23" s="3">
-        <f t="shared" ref="AP23" si="39">V23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AP23" si="40">V23*100/SUM($O23:$X23)</f>
         <v>10.843230573971258</v>
       </c>
       <c r="AQ23" s="3">
-        <f t="shared" ref="AQ23" si="40">W23*100/SUM($O23:$X23)</f>
+        <f t="shared" ref="AQ23" si="41">W23*100/SUM($O23:$X23)</f>
         <v>11.836776201309821</v>
       </c>
       <c r="AR23" s="3">
-        <f>X23*100/SUM($O23:$X23)</f>
+        <f t="shared" si="22"/>
         <v>23.017600799085354</v>
       </c>
     </row>
@@ -7890,11 +8133,11 @@
       </c>
       <c r="B24" s="17">
         <f>mtl_newcases!C25</f>
-        <v>4630</v>
+        <v>4628</v>
       </c>
       <c r="C24" s="17">
         <f>mtl_newcases!B25</f>
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D24">
         <v>63</v>
@@ -7971,83 +8214,83 @@
         <v>555.63989676635799</v>
       </c>
       <c r="Y24" s="3">
-        <f t="shared" ref="Y24" si="41">E24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="Y24" si="42">E24*100/SUM($E24:$N24)</f>
         <v>0.68243858052775253</v>
       </c>
       <c r="Z24" s="3">
-        <f t="shared" ref="Z24" si="42">F24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="Z24" si="43">F24*100/SUM($E24:$N24)</f>
         <v>0.70518653321201097</v>
       </c>
       <c r="AA24" s="3">
-        <f t="shared" ref="AA24" si="43">G24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AA24" si="44">G24*100/SUM($E24:$N24)</f>
         <v>3.5031847133757963</v>
       </c>
       <c r="AB24" s="3">
-        <f t="shared" ref="AB24" si="44">H24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AB24" si="45">H24*100/SUM($E24:$N24)</f>
         <v>15.059144676979072</v>
       </c>
       <c r="AC24" s="3">
-        <f t="shared" ref="AC24" si="45">I24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AC24" si="46">I24*100/SUM($E24:$N24)</f>
         <v>16.674249317561419</v>
       </c>
       <c r="AD24" s="3">
-        <f t="shared" ref="AD24" si="46">J24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AD24" si="47">J24*100/SUM($E24:$N24)</f>
         <v>17.356687898089174</v>
       </c>
       <c r="AE24" s="3">
-        <f t="shared" ref="AE24" si="47">K24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AE24" si="48">K24*100/SUM($E24:$N24)</f>
         <v>15.127388535031848</v>
       </c>
       <c r="AF24" s="3">
-        <f t="shared" ref="AF24" si="48">L24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AF24" si="49">L24*100/SUM($E24:$N24)</f>
         <v>10.668789808917197</v>
       </c>
       <c r="AG24" s="3">
-        <f t="shared" ref="AG24" si="49">M24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AG24" si="50">M24*100/SUM($E24:$N24)</f>
         <v>7.7343039126478619</v>
       </c>
       <c r="AH24" s="3">
-        <f t="shared" ref="AH24" si="50">N24*100/SUM($E24:$N24)</f>
+        <f t="shared" ref="AH24" si="51">N24*100/SUM($E24:$N24)</f>
         <v>12.48862602365787</v>
       </c>
       <c r="AI24" s="3">
-        <f t="shared" ref="AI24" si="51">O24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AI24" si="52">O24*100/SUM($O24:$X24)</f>
         <v>0.52752287287092714</v>
       </c>
       <c r="AJ24" s="3">
-        <f t="shared" ref="AJ24" si="52">P24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AJ24" si="53">P24*100/SUM($O24:$X24)</f>
         <v>1.3518663266268462</v>
       </c>
       <c r="AK24" s="3">
-        <f t="shared" ref="AK24" si="53">Q24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AK24" si="54">Q24*100/SUM($O24:$X24)</f>
         <v>3.7251680513018282</v>
       </c>
       <c r="AL24" s="3">
-        <f t="shared" ref="AL24" si="54">R24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AL24" si="55">R24*100/SUM($O24:$X24)</f>
         <v>10.277018696561045</v>
       </c>
       <c r="AM24" s="3">
-        <f t="shared" ref="AM24" si="55">S24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AM24" si="56">S24*100/SUM($O24:$X24)</f>
         <v>11.134317795689789</v>
       </c>
       <c r="AN24" s="3">
-        <f t="shared" ref="AN24" si="56">T24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AN24" si="57">T24*100/SUM($O24:$X24)</f>
         <v>13.64864591467845</v>
       </c>
       <c r="AO24" s="3">
-        <f t="shared" ref="AO24" si="57">U24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AO24" si="58">U24*100/SUM($O24:$X24)</f>
         <v>11.693423681972218</v>
       </c>
       <c r="AP24" s="3">
-        <f t="shared" ref="AP24" si="58">V24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AP24" si="59">V24*100/SUM($O24:$X24)</f>
         <v>10.414023212780554</v>
       </c>
       <c r="AQ24" s="3">
-        <f t="shared" ref="AQ24" si="59">W24*100/SUM($O24:$X24)</f>
+        <f t="shared" ref="AQ24" si="60">W24*100/SUM($O24:$X24)</f>
         <v>11.934825329764765</v>
       </c>
       <c r="AR24" s="3">
-        <f>X24*100/SUM($O24:$X24)</f>
+        <f t="shared" si="22"/>
         <v>25.293188117753569</v>
       </c>
     </row>
@@ -8057,7 +8300,7 @@
       </c>
       <c r="B25" s="17">
         <f>mtl_newcases!C26</f>
-        <v>5052</v>
+        <v>5050</v>
       </c>
       <c r="C25" s="17">
         <f>mtl_newcases!B26</f>
@@ -8138,83 +8381,83 @@
         <v>653.81306614037749</v>
       </c>
       <c r="Y25" s="3">
-        <f t="shared" ref="Y25" si="60">E25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="Y25" si="61">E25*100/SUM($E25:$N25)</f>
         <v>0.71368597816960533</v>
       </c>
       <c r="Z25" s="3">
-        <f t="shared" ref="Z25" si="61">F25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="Z25" si="62">F25*100/SUM($E25:$N25)</f>
         <v>0.69269521410579349</v>
       </c>
       <c r="AA25" s="3">
-        <f t="shared" ref="AA25" si="62">G25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AA25" si="63">G25*100/SUM($E25:$N25)</f>
         <v>3.4634760705289671</v>
       </c>
       <c r="AB25" s="3">
-        <f t="shared" ref="AB25" si="63">H25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AB25" si="64">H25*100/SUM($E25:$N25)</f>
         <v>14.609571788413099</v>
       </c>
       <c r="AC25" s="3">
-        <f t="shared" ref="AC25" si="64">I25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AC25" si="65">I25*100/SUM($E25:$N25)</f>
         <v>16.204869857262803</v>
       </c>
       <c r="AD25" s="3">
-        <f t="shared" ref="AD25" si="65">J25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AD25" si="66">J25*100/SUM($E25:$N25)</f>
         <v>17.569269521410579</v>
       </c>
       <c r="AE25" s="3">
-        <f t="shared" ref="AE25" si="66">K25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AE25" si="67">K25*100/SUM($E25:$N25)</f>
         <v>14.861460957178842</v>
       </c>
       <c r="AF25" s="3">
-        <f t="shared" ref="AF25" si="67">L25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AF25" si="68">L25*100/SUM($E25:$N25)</f>
         <v>10.600335852225021</v>
       </c>
       <c r="AG25" s="3">
-        <f t="shared" ref="AG25" si="68">M25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AG25" si="69">M25*100/SUM($E25:$N25)</f>
         <v>7.7246011754827872</v>
       </c>
       <c r="AH25" s="3">
-        <f t="shared" ref="AH25" si="69">N25*100/SUM($E25:$N25)</f>
+        <f t="shared" ref="AH25" si="70">N25*100/SUM($E25:$N25)</f>
         <v>13.560033585222502</v>
       </c>
       <c r="AI25" s="3">
-        <f t="shared" ref="AI25" si="70">O25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AI25" si="71">O25*100/SUM($O25:$X25)</f>
         <v>0.68612889377915209</v>
       </c>
       <c r="AJ25" s="3">
-        <f t="shared" ref="AJ25" si="71">P25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AJ25" si="72">P25*100/SUM($O25:$X25)</f>
         <v>1.3078775623282131</v>
       </c>
       <c r="AK25" s="3">
-        <f t="shared" ref="AK25" si="72">Q25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AK25" si="73">Q25*100/SUM($O25:$X25)</f>
         <v>3.6273560417575919</v>
       </c>
       <c r="AL25" s="3">
-        <f t="shared" ref="AL25" si="73">R25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AL25" si="74">R25*100/SUM($O25:$X25)</f>
         <v>9.8197287059184415</v>
       </c>
       <c r="AM25" s="3">
-        <f t="shared" ref="AM25" si="74">S25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AM25" si="75">S25*100/SUM($O25:$X25)</f>
         <v>10.657566008962512</v>
       </c>
       <c r="AN25" s="3">
-        <f t="shared" ref="AN25" si="75">T25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AN25" si="76">T25*100/SUM($O25:$X25)</f>
         <v>13.607288094695107</v>
       </c>
       <c r="AO25" s="3">
-        <f t="shared" ref="AO25" si="76">U25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AO25" si="77">U25*100/SUM($O25:$X25)</f>
         <v>11.314474569192503</v>
       </c>
       <c r="AP25" s="3">
-        <f t="shared" ref="AP25" si="77">V25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AP25" si="78">V25*100/SUM($O25:$X25)</f>
         <v>10.191032098778582</v>
       </c>
       <c r="AQ25" s="3">
-        <f t="shared" ref="AQ25" si="78">W25*100/SUM($O25:$X25)</f>
+        <f t="shared" ref="AQ25" si="79">W25*100/SUM($O25:$X25)</f>
         <v>11.739944983094992</v>
       </c>
       <c r="AR25" s="3">
-        <f>X25*100/SUM($O25:$X25)</f>
+        <f t="shared" si="22"/>
         <v>27.048603041492903</v>
       </c>
     </row>
@@ -8224,11 +8467,11 @@
       </c>
       <c r="B26" s="17">
         <f>mtl_newcases!C27</f>
-        <v>5262</v>
+        <v>5403</v>
       </c>
       <c r="C26" s="17">
         <f>mtl_newcases!B27</f>
-        <v>210</v>
+        <v>353</v>
       </c>
       <c r="D26">
         <v>91</v>
@@ -8305,83 +8548,83 @@
         <v>767.16765345883312</v>
       </c>
       <c r="Y26" s="3">
-        <f t="shared" ref="Y26" si="79">E26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="Y26" si="80">E26*100/SUM($E26:$N26)</f>
         <v>0.68597560975609762</v>
       </c>
       <c r="Z26" s="3">
-        <f t="shared" ref="Z26" si="80">F26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="Z26" si="81">F26*100/SUM($E26:$N26)</f>
         <v>0.62881097560975607</v>
       </c>
       <c r="AA26" s="3">
-        <f t="shared" ref="AA26" si="81">G26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AA26" si="82">G26*100/SUM($E26:$N26)</f>
         <v>3.2583841463414633</v>
       </c>
       <c r="AB26" s="3">
-        <f t="shared" ref="AB26" si="82">H26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AB26" si="83">H26*100/SUM($E26:$N26)</f>
         <v>14.310213414634147</v>
       </c>
       <c r="AC26" s="3">
-        <f t="shared" ref="AC26" si="83">I26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AC26" si="84">I26*100/SUM($E26:$N26)</f>
         <v>16.120426829268293</v>
       </c>
       <c r="AD26" s="3">
-        <f t="shared" ref="AD26" si="84">J26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AD26" si="85">J26*100/SUM($E26:$N26)</f>
         <v>17.301829268292682</v>
       </c>
       <c r="AE26" s="3">
-        <f t="shared" ref="AE26" si="85">K26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AE26" si="86">K26*100/SUM($E26:$N26)</f>
         <v>14.691310975609756</v>
       </c>
       <c r="AF26" s="3">
-        <f t="shared" ref="AF26" si="86">L26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AF26" si="87">L26*100/SUM($E26:$N26)</f>
         <v>10.499237804878049</v>
       </c>
       <c r="AG26" s="3">
-        <f t="shared" ref="AG26" si="87">M26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AG26" si="88">M26*100/SUM($E26:$N26)</f>
         <v>8.0602134146341466</v>
       </c>
       <c r="AH26" s="3">
-        <f t="shared" ref="AH26" si="88">N26*100/SUM($E26:$N26)</f>
+        <f t="shared" ref="AH26" si="89">N26*100/SUM($E26:$N26)</f>
         <v>14.44359756097561</v>
       </c>
       <c r="AI26" s="3">
-        <f t="shared" ref="AI26" si="89">O26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AI26" si="90">O26*100/SUM($O26:$X26)</f>
         <v>1.0261064481957152</v>
       </c>
       <c r="AJ26" s="3">
-        <f t="shared" ref="AJ26" si="90">P26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AJ26" si="91">P26*100/SUM($O26:$X26)</f>
         <v>1.1685270283264069</v>
       </c>
       <c r="AK26" s="3">
-        <f t="shared" ref="AK26" si="91">Q26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AK26" si="92">Q26*100/SUM($O26:$X26)</f>
         <v>3.3587217363742949</v>
       </c>
       <c r="AL26" s="3">
-        <f t="shared" ref="AL26" si="92">R26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AL26" si="93">R26*100/SUM($O26:$X26)</f>
         <v>9.4667707425770207</v>
       </c>
       <c r="AM26" s="3">
-        <f t="shared" ref="AM26" si="93">S26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AM26" si="94">S26*100/SUM($O26:$X26)</f>
         <v>10.434767260356979</v>
       </c>
       <c r="AN26" s="3">
-        <f t="shared" ref="AN26" si="94">T26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AN26" si="95">T26*100/SUM($O26:$X26)</f>
         <v>13.188750221636536</v>
       </c>
       <c r="AO26" s="3">
-        <f t="shared" ref="AO26" si="95">U26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AO26" si="96">U26*100/SUM($O26:$X26)</f>
         <v>11.008475596304274</v>
       </c>
       <c r="AP26" s="3">
-        <f t="shared" ref="AP26" si="96">V26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AP26" si="97">V26*100/SUM($O26:$X26)</f>
         <v>9.934592624477073</v>
       </c>
       <c r="AQ26" s="3">
-        <f t="shared" ref="AQ26" si="97">W26*100/SUM($O26:$X26)</f>
+        <f t="shared" ref="AQ26" si="98">W26*100/SUM($O26:$X26)</f>
         <v>12.056750766299654</v>
       </c>
       <c r="AR26" s="3">
-        <f>X26*100/SUM($O26:$X26)</f>
+        <f t="shared" si="22"/>
         <v>28.356537575452048</v>
       </c>
     </row>
@@ -8395,131 +8638,161 @@
       </c>
       <c r="C27" s="17">
         <f>mtl_newcases!B28</f>
-        <v>355</v>
+        <v>214</v>
       </c>
       <c r="D27">
         <v>100</v>
       </c>
-      <c r="E27" t="str" cm="1">
+      <c r="E27" cm="1">
         <f t="array" ref="E27:N27">TRANSPOSE(santemontreal!L$57:L$66)</f>
-        <v>na</v>
-      </c>
-      <c r="F27" t="str">
-        <v>na</v>
-      </c>
-      <c r="G27" t="str">
-        <v>na</v>
-      </c>
-      <c r="H27" t="str">
-        <v>na</v>
-      </c>
-      <c r="I27" t="str">
-        <v>na</v>
-      </c>
-      <c r="J27" t="str">
-        <v>na</v>
-      </c>
-      <c r="K27" t="str">
-        <v>na</v>
-      </c>
-      <c r="L27" t="str">
-        <v>na</v>
-      </c>
-      <c r="M27" t="str">
-        <v>na</v>
-      </c>
-      <c r="N27" t="str">
-        <v>na</v>
-      </c>
-      <c r="O27" t="s">
-        <v>102</v>
-      </c>
-      <c r="P27" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>102</v>
-      </c>
-      <c r="R27" t="s">
-        <v>102</v>
-      </c>
-      <c r="S27" t="s">
-        <v>102</v>
-      </c>
-      <c r="T27" t="s">
-        <v>102</v>
-      </c>
-      <c r="U27" t="s">
-        <v>102</v>
-      </c>
-      <c r="V27" t="s">
-        <v>102</v>
-      </c>
-      <c r="W27" t="s">
-        <v>102</v>
-      </c>
-      <c r="X27" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AL27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ27" t="s">
-        <v>102</v>
-      </c>
-      <c r="AR27" t="s">
-        <v>102</v>
+        <v>37</v>
+      </c>
+      <c r="F27">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <v>177</v>
+      </c>
+      <c r="H27">
+        <v>783</v>
+      </c>
+      <c r="I27">
+        <v>887</v>
+      </c>
+      <c r="J27">
+        <v>966</v>
+      </c>
+      <c r="K27">
+        <v>828</v>
+      </c>
+      <c r="L27">
+        <v>581</v>
+      </c>
+      <c r="M27">
+        <v>446</v>
+      </c>
+      <c r="N27">
+        <v>862</v>
+      </c>
+      <c r="O27" s="18">
+        <f>E27/(age_distribution_2016!$B11/100000)</f>
+        <v>37.44749759627549</v>
+      </c>
+      <c r="P27" s="18">
+        <f>F27/(age_distribution_2016!$B$3/100000)</f>
+        <v>32.571729654643867</v>
+      </c>
+      <c r="Q27" s="18">
+        <f>G27/(age_distribution_2016!$B$4/100000)</f>
+        <v>94.056380689215402</v>
+      </c>
+      <c r="R27" s="18">
+        <f>H27/(age_distribution_2016!$B$5/100000)</f>
+        <v>267.03043737744053</v>
+      </c>
+      <c r="S27" s="18">
+        <f>I27/(age_distribution_2016!$B$6/100000)</f>
+        <v>295.98731959622927</v>
+      </c>
+      <c r="T27" s="18">
+        <f>J27/(age_distribution_2016!$B$7/100000)</f>
+        <v>379.60506926024169</v>
+      </c>
+      <c r="U27" s="18">
+        <f>K27/(age_distribution_2016!$B$8/100000)</f>
+        <v>319.84548527281504</v>
+      </c>
+      <c r="V27" s="18">
+        <f>L27/(age_distribution_2016!$B$9/100000)</f>
+        <v>283.4077217628838</v>
+      </c>
+      <c r="W27" s="18">
+        <f>M27/(age_distribution_2016!$B$10/100000)</f>
+        <v>343.92350400987044</v>
+      </c>
+      <c r="X27" s="18">
+        <f>N27/(age_distribution_2016!$B$11/100000)</f>
+        <v>872.42548454025609</v>
+      </c>
+      <c r="Y27" s="3">
+        <f t="shared" ref="Y27" si="99">E27*100/SUM($E27:$N27)</f>
+        <v>0.66059632208534191</v>
+      </c>
+      <c r="Z27" s="3">
+        <f t="shared" ref="Z27" si="100">F27*100/SUM($E27:$N27)</f>
+        <v>0.60703445813247636</v>
+      </c>
+      <c r="AA27" s="3">
+        <f t="shared" ref="AA27" si="101">G27*100/SUM($E27:$N27)</f>
+        <v>3.1601499732190681</v>
+      </c>
+      <c r="AB27" s="3">
+        <f t="shared" ref="AB27" si="102">H27*100/SUM($E27:$N27)</f>
+        <v>13.979646491697912</v>
+      </c>
+      <c r="AC27" s="3">
+        <f t="shared" ref="AC27" si="103">I27*100/SUM($E27:$N27)</f>
+        <v>15.83645777539725</v>
+      </c>
+      <c r="AD27" s="3">
+        <f t="shared" ref="AD27" si="104">J27*100/SUM($E27:$N27)</f>
+        <v>17.24692019282271</v>
+      </c>
+      <c r="AE27" s="3">
+        <f t="shared" ref="AE27" si="105">K27*100/SUM($E27:$N27)</f>
+        <v>14.783074450990895</v>
+      </c>
+      <c r="AF27" s="3">
+        <f t="shared" ref="AF27" si="106">L27*100/SUM($E27:$N27)</f>
+        <v>10.373147652204963</v>
+      </c>
+      <c r="AG27" s="3">
+        <f t="shared" ref="AG27" si="107">M27*100/SUM($E27:$N27)</f>
+        <v>7.9628637743260136</v>
+      </c>
+      <c r="AH27" s="3">
+        <f t="shared" ref="AH27" si="108">N27*100/SUM($E27:$N27)</f>
+        <v>15.39010890912337</v>
+      </c>
+      <c r="AI27" s="3">
+        <f t="shared" ref="AI27" si="109">O27*100/SUM($O27:$X27)</f>
+        <v>1.2796873026456062</v>
+      </c>
+      <c r="AJ27" s="3">
+        <f t="shared" ref="AJ27" si="110">P27*100/SUM($O27:$X27)</f>
+        <v>1.1130684702520348</v>
+      </c>
+      <c r="AK27" s="3">
+        <f t="shared" ref="AK27" si="111">Q27*100/SUM($O27:$X27)</f>
+        <v>3.2141735450104298</v>
+      </c>
+      <c r="AL27" s="3">
+        <f t="shared" ref="AL27" si="112">R27*100/SUM($O27:$X27)</f>
+        <v>9.1251881184658963</v>
+      </c>
+      <c r="AM27" s="3">
+        <f t="shared" ref="AM27" si="113">S27*100/SUM($O27:$X27)</f>
+        <v>10.11472698963666</v>
+      </c>
+      <c r="AN27" s="3">
+        <f t="shared" ref="AN27" si="114">T27*100/SUM($O27:$X27)</f>
+        <v>12.972182878264002</v>
+      </c>
+      <c r="AO27" s="3">
+        <f t="shared" ref="AO27" si="115">U27*100/SUM($O27:$X27)</f>
+        <v>10.93002824180307</v>
+      </c>
+      <c r="AP27" s="3">
+        <f t="shared" ref="AP27" si="116">V27*100/SUM($O27:$X27)</f>
+        <v>9.6848464194240993</v>
+      </c>
+      <c r="AQ27" s="3">
+        <f t="shared" ref="AQ27" si="117">W27*100/SUM($O27:$X27)</f>
+        <v>11.752842497187048</v>
+      </c>
+      <c r="AR27" s="3">
+        <f t="shared" si="22"/>
+        <v>29.813255537311154</v>
       </c>
     </row>
   </sheetData>
@@ -9453,7 +9726,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9710,11 +9983,11 @@
         <v>43921</v>
       </c>
       <c r="B19">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="E19" s="19">
         <v>43921</v>
@@ -9724,7 +9997,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -9736,7 +10009,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="E20" s="19">
         <v>43922</v>
@@ -9746,7 +10019,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -9758,7 +10031,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>3244</v>
+        <v>3243</v>
       </c>
       <c r="E21" s="19">
         <v>43923</v>
@@ -9768,7 +10041,7 @@
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G26" si="2">C21-F21</f>
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -9780,7 +10053,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>3609</v>
+        <v>3608</v>
       </c>
       <c r="E22" s="19">
         <v>43924</v>
@@ -9790,7 +10063,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -9802,7 +10075,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>3932</v>
+        <v>3931</v>
       </c>
       <c r="E23" s="19">
         <v>43925</v>
@@ -9812,7 +10085,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -9824,7 +10097,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>4196</v>
+        <v>4195</v>
       </c>
       <c r="E24" s="19">
         <v>43926</v>
@@ -9834,7 +10107,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -9842,11 +10115,11 @@
         <v>43927</v>
       </c>
       <c r="B25">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>4630</v>
+        <v>4628</v>
       </c>
       <c r="E25" s="19">
         <v>43927</v>
@@ -9856,7 +10129,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -9868,7 +10141,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>5052</v>
+        <v>5050</v>
       </c>
       <c r="E26" s="19">
         <v>43928</v>
@@ -9878,7 +10151,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -9886,11 +10159,11 @@
         <v>43929</v>
       </c>
       <c r="B27">
-        <v>210</v>
+        <v>353</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>5262</v>
+        <v>5403</v>
       </c>
       <c r="E27" s="19">
         <v>43929</v>
@@ -9900,7 +10173,7 @@
       </c>
       <c r="G27">
         <f t="shared" ref="G27:G28" si="3">C27-F27</f>
-        <v>0</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -9908,7 +10181,7 @@
         <v>43930</v>
       </c>
       <c r="B28">
-        <v>355</v>
+        <v>214</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
@@ -9935,8 +10208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E261AEA-18EA-4FE9-ACAC-1FB61BEBD535}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N66" sqref="N66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L35" sqref="L2:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9979,10 +10252,10 @@
         <v>236</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -10023,8 +10296,8 @@
       <c r="K2" s="7">
         <v>247</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>102</v>
+      <c r="L2" s="7">
+        <v>277</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -10065,8 +10338,8 @@
       <c r="K3" s="9">
         <v>59</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>102</v>
+      <c r="L3" s="9">
+        <v>67</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
@@ -10107,8 +10380,8 @@
       <c r="K4" s="7">
         <v>5</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>102</v>
+      <c r="L4" s="7">
+        <v>5</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -10149,8 +10422,8 @@
       <c r="K5" s="9">
         <v>14</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>102</v>
+      <c r="L5" s="9">
+        <v>14</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -10191,8 +10464,8 @@
       <c r="K6" s="7">
         <v>501</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>102</v>
+      <c r="L6" s="7">
+        <v>522</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -10233,8 +10506,8 @@
       <c r="K7" s="9">
         <v>262</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>102</v>
+      <c r="L7" s="9">
+        <v>264</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -10275,8 +10548,8 @@
       <c r="K8" s="7">
         <v>66</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>102</v>
+      <c r="L8" s="7">
+        <v>68</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -10317,8 +10590,8 @@
       <c r="K9" s="9">
         <v>37</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>102</v>
+      <c r="L9" s="9">
+        <v>37</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -10359,8 +10632,8 @@
       <c r="K10" s="7">
         <v>29</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>102</v>
+      <c r="L10" s="7">
+        <v>29</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -10401,8 +10674,8 @@
       <c r="K11" s="9">
         <v>14</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>102</v>
+      <c r="L11" s="9">
+        <v>15</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -10443,8 +10716,8 @@
       <c r="K12" s="7">
         <v>83</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>102</v>
+      <c r="L12" s="7">
+        <v>83</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -10485,8 +10758,8 @@
       <c r="K13" s="9">
         <v>286</v>
       </c>
-      <c r="L13" s="9" t="s">
-        <v>102</v>
+      <c r="L13" s="9">
+        <v>298</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -10527,8 +10800,8 @@
       <c r="K14" s="7">
         <v>19</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>102</v>
+      <c r="L14" s="7">
+        <v>22</v>
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -10569,8 +10842,8 @@
       <c r="K15" s="9">
         <v>213</v>
       </c>
-      <c r="L15" s="9" t="s">
-        <v>102</v>
+      <c r="L15" s="9">
+        <v>232</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -10611,8 +10884,8 @@
       <c r="K16" s="7">
         <v>6</v>
       </c>
-      <c r="L16" s="7" t="s">
-        <v>102</v>
+      <c r="L16" s="7">
+        <v>7</v>
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
@@ -10653,8 +10926,8 @@
       <c r="K17" s="9">
         <v>193</v>
       </c>
-      <c r="L17" s="9" t="s">
-        <v>102</v>
+      <c r="L17" s="9">
+        <v>238</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -10695,8 +10968,8 @@
       <c r="K18" s="7">
         <v>5</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>102</v>
+      <c r="L18" s="7">
+        <v>5</v>
       </c>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
@@ -10737,8 +11010,8 @@
       <c r="K19" s="9">
         <v>44</v>
       </c>
-      <c r="L19" s="9" t="s">
-        <v>102</v>
+      <c r="L19" s="9">
+        <v>44</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
@@ -10779,8 +11052,8 @@
       <c r="K20" s="7">
         <v>139</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>102</v>
+      <c r="L20" s="7">
+        <v>143</v>
       </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -10821,8 +11094,8 @@
       <c r="K21" s="9">
         <v>75</v>
       </c>
-      <c r="L21" s="9" t="s">
-        <v>102</v>
+      <c r="L21" s="9">
+        <v>78</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -10863,8 +11136,8 @@
       <c r="K22" s="7">
         <v>220</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>102</v>
+      <c r="L22" s="7">
+        <v>232</v>
       </c>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
@@ -10905,8 +11178,8 @@
       <c r="K23" s="9">
         <v>32</v>
       </c>
-      <c r="L23" s="9" t="s">
-        <v>102</v>
+      <c r="L23" s="9">
+        <v>33</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -10947,8 +11220,8 @@
       <c r="K24" s="7">
         <v>180</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>102</v>
+      <c r="L24" s="7">
+        <v>194</v>
       </c>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
@@ -10989,8 +11262,8 @@
       <c r="K25" s="9">
         <v>247</v>
       </c>
-      <c r="L25" s="9" t="s">
-        <v>102</v>
+      <c r="L25" s="9">
+        <v>260</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -11031,8 +11304,8 @@
       <c r="K26" s="7">
         <v>5</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>102</v>
+      <c r="L26" s="7">
+        <v>5</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -11073,8 +11346,8 @@
       <c r="K27" s="9">
         <v>163</v>
       </c>
-      <c r="L27" s="9" t="s">
-        <v>102</v>
+      <c r="L27" s="9">
+        <v>167</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -11115,8 +11388,8 @@
       <c r="K28" s="7">
         <v>124</v>
       </c>
-      <c r="L28" s="7" t="s">
-        <v>102</v>
+      <c r="L28" s="7">
+        <v>139</v>
       </c>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
@@ -11154,11 +11427,11 @@
       <c r="J29" s="20">
         <v>1</v>
       </c>
-      <c r="K29" s="9">
+      <c r="K29" s="20">
         <v>2</v>
       </c>
-      <c r="L29" s="9" t="s">
-        <v>102</v>
+      <c r="L29" s="20">
+        <v>2</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
@@ -11199,8 +11472,8 @@
       <c r="K30" s="7">
         <v>184</v>
       </c>
-      <c r="L30" s="7" t="s">
-        <v>102</v>
+      <c r="L30" s="7">
+        <v>210</v>
       </c>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
@@ -11241,8 +11514,8 @@
       <c r="K31" s="9">
         <v>154</v>
       </c>
-      <c r="L31" s="9" t="s">
-        <v>102</v>
+      <c r="L31" s="9">
+        <v>174</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
@@ -11283,8 +11556,8 @@
       <c r="K32" s="7">
         <v>174</v>
       </c>
-      <c r="L32" s="7" t="s">
-        <v>102</v>
+      <c r="L32" s="7">
+        <v>185</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
@@ -11325,8 +11598,8 @@
       <c r="K33" s="9">
         <v>242</v>
       </c>
-      <c r="L33" s="9" t="s">
-        <v>102</v>
+      <c r="L33" s="9">
+        <v>266</v>
       </c>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -11367,8 +11640,8 @@
       <c r="K34" s="7">
         <v>57</v>
       </c>
-      <c r="L34" s="7" t="s">
-        <v>102</v>
+      <c r="L34" s="7">
+        <v>57</v>
       </c>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
@@ -11409,8 +11682,8 @@
       <c r="K35" s="9">
         <v>1181</v>
       </c>
-      <c r="L35" s="9" t="s">
-        <v>102</v>
+      <c r="L35" s="9">
+        <v>1245</v>
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
@@ -11451,8 +11724,8 @@
       <c r="K36" s="11">
         <v>5262</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>102</v>
+      <c r="L36" s="11">
+        <v>5617</v>
       </c>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
@@ -11492,10 +11765,10 @@
         <v>236</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
@@ -11536,8 +11809,8 @@
       <c r="K39" s="7">
         <v>1145</v>
       </c>
-      <c r="L39" s="7" t="s">
-        <v>102</v>
+      <c r="L39" s="7">
+        <v>1178</v>
       </c>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
@@ -11578,8 +11851,8 @@
       <c r="K40" s="9">
         <v>673</v>
       </c>
-      <c r="L40" s="9" t="s">
-        <v>102</v>
+      <c r="L40" s="9">
+        <v>639</v>
       </c>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
@@ -11620,8 +11893,8 @@
       <c r="K41" s="7">
         <v>827</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>102</v>
+      <c r="L41" s="7">
+        <v>908</v>
       </c>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
@@ -11662,8 +11935,8 @@
       <c r="K42" s="9">
         <v>788</v>
       </c>
-      <c r="L42" s="9" t="s">
-        <v>102</v>
+      <c r="L42" s="9">
+        <v>877</v>
       </c>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
@@ -11704,8 +11977,8 @@
       <c r="K43" s="7">
         <v>639</v>
       </c>
-      <c r="L43" s="7" t="s">
-        <v>102</v>
+      <c r="L43" s="7">
+        <v>661</v>
       </c>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
@@ -11746,8 +12019,8 @@
       <c r="K44" s="9">
         <v>1190</v>
       </c>
-      <c r="L44" s="9" t="s">
-        <v>102</v>
+      <c r="L44" s="9">
+        <v>1254</v>
       </c>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
@@ -11788,8 +12061,8 @@
       <c r="K45" s="11">
         <v>5262</v>
       </c>
-      <c r="L45" s="7" t="s">
-        <v>102</v>
+      <c r="L45" s="11">
+        <v>5617</v>
       </c>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
@@ -11827,10 +12100,10 @@
         <v>236</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
@@ -11867,10 +12140,10 @@
         <v>230</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>102</v>
+        <v>245</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -11907,10 +12180,10 @@
         <v>231</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
@@ -11947,10 +12220,10 @@
         <v>232</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="L50" s="7" t="s">
-        <v>102</v>
+        <v>241</v>
+      </c>
+      <c r="L50" s="7">
+        <v>167.4</v>
       </c>
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
@@ -11987,10 +12260,10 @@
         <v>233</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>102</v>
+        <v>249</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
@@ -12027,10 +12300,10 @@
         <v>234</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>102</v>
+        <v>250</v>
       </c>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
@@ -12054,7 +12327,7 @@
         <v>235</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
@@ -12089,10 +12362,10 @@
       </c>
       <c r="J54" s="7"/>
       <c r="K54" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L54" s="7" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
@@ -12130,10 +12403,10 @@
         <v>236</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="M56" s="13"/>
       <c r="N56" s="13"/>
@@ -12172,8 +12445,8 @@
       <c r="K57" s="7">
         <v>36</v>
       </c>
-      <c r="L57" s="7" t="s">
-        <v>102</v>
+      <c r="L57" s="7">
+        <v>37</v>
       </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
@@ -12212,8 +12485,8 @@
       <c r="K58" s="9">
         <v>33</v>
       </c>
-      <c r="L58" s="9" t="s">
-        <v>102</v>
+      <c r="L58" s="9">
+        <v>34</v>
       </c>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
@@ -12252,8 +12525,8 @@
       <c r="K59" s="7">
         <v>171</v>
       </c>
-      <c r="L59" s="7" t="s">
-        <v>102</v>
+      <c r="L59" s="7">
+        <v>177</v>
       </c>
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
@@ -12292,8 +12565,8 @@
       <c r="K60" s="9">
         <v>751</v>
       </c>
-      <c r="L60" s="9" t="s">
-        <v>102</v>
+      <c r="L60" s="9">
+        <v>783</v>
       </c>
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
@@ -12332,8 +12605,8 @@
       <c r="K61" s="7">
         <v>846</v>
       </c>
-      <c r="L61" s="7" t="s">
-        <v>102</v>
+      <c r="L61" s="7">
+        <v>887</v>
       </c>
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
@@ -12372,8 +12645,8 @@
       <c r="K62" s="9">
         <v>908</v>
       </c>
-      <c r="L62" s="9" t="s">
-        <v>102</v>
+      <c r="L62" s="9">
+        <v>966</v>
       </c>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
@@ -12412,8 +12685,8 @@
       <c r="K63" s="7">
         <v>771</v>
       </c>
-      <c r="L63" s="7" t="s">
-        <v>102</v>
+      <c r="L63" s="7">
+        <v>828</v>
       </c>
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
@@ -12452,8 +12725,8 @@
       <c r="K64" s="9">
         <v>551</v>
       </c>
-      <c r="L64" s="9" t="s">
-        <v>102</v>
+      <c r="L64" s="9">
+        <v>581</v>
       </c>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
@@ -12492,8 +12765,8 @@
       <c r="K65" s="7">
         <v>423</v>
       </c>
-      <c r="L65" s="7" t="s">
-        <v>102</v>
+      <c r="L65" s="7">
+        <v>446</v>
       </c>
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
@@ -12532,8 +12805,8 @@
       <c r="K66" s="9">
         <v>758</v>
       </c>
-      <c r="L66" s="9" t="s">
-        <v>102</v>
+      <c r="L66" s="9">
+        <v>862</v>
       </c>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
@@ -12572,8 +12845,8 @@
       <c r="K67" s="7">
         <v>14</v>
       </c>
-      <c r="L67" s="7" t="s">
-        <v>102</v>
+      <c r="L67" s="7">
+        <v>16</v>
       </c>
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
@@ -12613,7 +12886,7 @@
         <v>5262</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>102</v>
+        <v>251</v>
       </c>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
@@ -12672,17 +12945,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655ECF0F-EC0D-4FC9-B182-78DF99BFDAD7}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B10"/>
+      <selection activeCell="B4" sqref="B4:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
         <v>228</v>
@@ -12693,141 +12966,507 @@
       <c r="D1" t="s">
         <v>183</v>
       </c>
-      <c r="E1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <v>522</v>
+      </c>
+      <c r="C8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9">
+        <v>264</v>
+      </c>
+      <c r="C9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>277</v>
+      </c>
+      <c r="D12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>298</v>
+      </c>
+      <c r="C15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>285</v>
+      </c>
+      <c r="D16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>232</v>
+      </c>
+      <c r="C17" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>238</v>
+      </c>
+      <c r="C19" t="s">
+        <v>292</v>
+      </c>
+      <c r="D19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>260</v>
+      </c>
+      <c r="D20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>296</v>
+      </c>
+      <c r="D21">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22">
+        <v>143</v>
+      </c>
+      <c r="C22" t="s">
+        <v>297</v>
+      </c>
+      <c r="D22">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>298</v>
+      </c>
+      <c r="D23" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <v>232</v>
+      </c>
+      <c r="C24" t="s">
+        <v>287</v>
+      </c>
+      <c r="D24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>301</v>
+      </c>
+      <c r="B25">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>302</v>
+      </c>
+      <c r="D25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26">
+        <v>194</v>
+      </c>
+      <c r="C26" t="s">
+        <v>304</v>
+      </c>
+      <c r="D26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27">
+        <v>260</v>
+      </c>
+      <c r="C27" t="s">
+        <v>306</v>
+      </c>
+      <c r="D27" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29">
+        <v>167</v>
+      </c>
+      <c r="C29" t="s">
+        <v>309</v>
+      </c>
+      <c r="D29" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>311</v>
+      </c>
+      <c r="D30" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32">
+        <v>210</v>
+      </c>
+      <c r="C32" t="s">
+        <v>314</v>
+      </c>
+      <c r="D32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33">
+        <v>174</v>
+      </c>
+      <c r="C33" t="s">
+        <v>316</v>
+      </c>
+      <c r="D33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34">
+        <v>185</v>
+      </c>
+      <c r="C34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D34" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35">
+        <v>266</v>
+      </c>
+      <c r="C35" t="s">
+        <v>320</v>
+      </c>
+      <c r="D35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>322</v>
+      </c>
+      <c r="B36">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>323</v>
+      </c>
+      <c r="D36" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>247</v>
       </c>
-      <c r="C4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5">
-        <v>639</v>
-      </c>
-      <c r="C5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B37" t="s">
+        <v>325</v>
+      </c>
+      <c r="C37" t="s">
+        <v>235</v>
+      </c>
+      <c r="D37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>326</v>
+      </c>
+      <c r="B38" t="s">
         <v>251</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6">
-        <v>908</v>
-      </c>
-      <c r="C6">
-        <v>20.8</v>
-      </c>
-      <c r="D6">
-        <v>167.4</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7">
-        <v>788</v>
-      </c>
-      <c r="C7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D7" t="s">
-        <v>243</v>
-      </c>
-      <c r="E7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8">
-        <v>639</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C38" t="s">
+        <v>235</v>
+      </c>
+      <c r="D38" t="s">
         <v>253</v>
       </c>
-      <c r="D8" t="s">
-        <v>244</v>
-      </c>
-      <c r="E8">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>254</v>
-      </c>
-      <c r="B9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" t="s">
-        <v>235</v>
-      </c>
-      <c r="D9" t="s">
-        <v>235</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" t="s">
-        <v>235</v>
-      </c>
-      <c r="D10" t="s">
-        <v>245</v>
-      </c>
-      <c r="E10">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update data (2020-04-20), partial MTL data
Data for Number of cases per Montreal borough and by age group were not released for 2020-04-19. Complete data for QC were released.
</commit_message>
<xml_diff>
--- a/data/covid19_MTL.xlsx
+++ b/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B468453D-6FB0-4A2E-BC24-61B2FFAEA536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B909654-AB5A-4F75-82CF-A42EAD9C32D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18040" yWindow="3870" windowWidth="36930" windowHeight="16890" tabRatio="765" activeTab="3" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="11370" yWindow="6290" windowWidth="29840" windowHeight="14430" tabRatio="512" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="306">
   <si>
     <t>borough</t>
   </si>
@@ -990,6 +990,9 @@
   <si>
     <t>1 671,6</t>
   </si>
+  <si>
+    <t>19 AVRIL, 17H15</t>
+  </si>
 </sst>
 </file>
 
@@ -1130,7 +1133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1186,6 +1189,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1500,20 +1504,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5D96B4-0147-4A32-9FAF-C932A9839F40}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="42.453125" customWidth="1"/>
     <col min="2" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1580,8 +1584,11 @@
       <c r="V1" s="1">
         <v>43939</v>
       </c>
+      <c r="W1" s="1">
+        <v>43940</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1648,8 +1655,11 @@
       <c r="V2">
         <v>663</v>
       </c>
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1716,8 +1726,11 @@
       <c r="V3">
         <v>138</v>
       </c>
+      <c r="W3" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1784,8 +1797,11 @@
       <c r="V4">
         <v>5</v>
       </c>
+      <c r="W4" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1852,8 +1868,11 @@
       <c r="V5">
         <v>15</v>
       </c>
+      <c r="W5" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1920,8 +1939,11 @@
       <c r="V6">
         <v>839</v>
       </c>
+      <c r="W6" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -1988,8 +2010,11 @@
       <c r="V7">
         <v>300</v>
       </c>
+      <c r="W7" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2056,8 +2081,11 @@
       <c r="V8">
         <v>96</v>
       </c>
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -2124,8 +2152,11 @@
       <c r="V9">
         <v>49</v>
       </c>
+      <c r="W9" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -2192,8 +2223,11 @@
       <c r="V10">
         <v>29</v>
       </c>
+      <c r="W10" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -2260,8 +2294,11 @@
       <c r="V11">
         <v>25</v>
       </c>
+      <c r="W11" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2328,8 +2365,11 @@
       <c r="V12">
         <v>108</v>
       </c>
+      <c r="W12" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2396,8 +2436,11 @@
       <c r="V13">
         <v>384</v>
       </c>
+      <c r="W13" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2464,8 +2507,11 @@
       <c r="V14">
         <v>31</v>
       </c>
+      <c r="W14" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2532,8 +2578,11 @@
       <c r="V15">
         <v>488</v>
       </c>
+      <c r="W15" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -2600,8 +2649,11 @@
       <c r="V16">
         <v>8</v>
       </c>
+      <c r="W16" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2668,8 +2720,11 @@
       <c r="V17">
         <v>577</v>
       </c>
+      <c r="W17" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -2736,8 +2791,11 @@
       <c r="V18">
         <v>6</v>
       </c>
+      <c r="W18" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -2804,8 +2862,11 @@
       <c r="V19">
         <v>63</v>
       </c>
+      <c r="W19" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2872,8 +2933,11 @@
       <c r="V20">
         <v>162</v>
       </c>
+      <c r="W20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2940,8 +3004,11 @@
       <c r="V21">
         <v>110</v>
       </c>
+      <c r="W21" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3008,8 +3075,11 @@
       <c r="V22">
         <v>363</v>
       </c>
+      <c r="W22" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -3076,8 +3146,11 @@
       <c r="V23">
         <v>40</v>
       </c>
+      <c r="W23" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3144,8 +3217,11 @@
       <c r="V24">
         <v>444</v>
       </c>
+      <c r="W24" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3212,8 +3288,11 @@
       <c r="V25">
         <v>418</v>
       </c>
+      <c r="W25" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -3280,8 +3359,11 @@
       <c r="V26">
         <v>5</v>
       </c>
+      <c r="W26" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3348,8 +3430,11 @@
       <c r="V27">
         <v>271</v>
       </c>
+      <c r="W27" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -3416,8 +3501,11 @@
       <c r="V28">
         <v>294</v>
       </c>
+      <c r="W28" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -3484,8 +3572,11 @@
       <c r="V29">
         <v>2</v>
       </c>
+      <c r="W29" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3552,8 +3643,11 @@
       <c r="V30">
         <v>350</v>
       </c>
+      <c r="W30" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3620,8 +3714,11 @@
       <c r="V31">
         <v>350</v>
       </c>
+      <c r="W31" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -3688,8 +3785,11 @@
       <c r="V32">
         <v>261</v>
       </c>
+      <c r="W32" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -3756,8 +3856,11 @@
       <c r="V33">
         <v>529</v>
       </c>
+      <c r="W33" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -3824,8 +3927,11 @@
       <c r="V34">
         <v>70</v>
       </c>
+      <c r="W34" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -3891,6 +3997,9 @@
       </c>
       <c r="V35">
         <v>964</v>
+      </c>
+      <c r="W35" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3901,20 +4010,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2135A11-D06E-4452-A066-9CB8F334EEDF}">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.08984375" customWidth="1"/>
     <col min="2" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="23" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4002,8 +4111,11 @@
         <f>cases!V1</f>
         <v>43939</v>
       </c>
+      <c r="W1" s="1">
+        <v>43940</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4090,8 +4202,11 @@
         <f>cases!V2/(population_2016!$B2/1000)</f>
         <v>4.9387314238891573</v>
       </c>
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4178,8 +4293,11 @@
         <f>cases!V3/(population_2016!$B3/1000)</f>
         <v>3.2246004299467241</v>
       </c>
+      <c r="W3" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -4266,8 +4384,11 @@
         <f>cases!V4/(population_2016!$B4/1000)</f>
         <v>1.3078733978550876</v>
       </c>
+      <c r="W4" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -4354,8 +4475,11 @@
         <f>cases!V5/(population_2016!$B5/1000)</f>
         <v>0.77623680397433237</v>
       </c>
+      <c r="W5" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4442,8 +4566,11 @@
         <f>cases!V6/(population_2016!$B6/1000)</f>
         <v>5.0384338217631512</v>
       </c>
+      <c r="W6" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -4530,8 +4657,11 @@
         <f>cases!V7/(population_2016!$B7/1000)</f>
         <v>9.2455621301775146</v>
       </c>
+      <c r="W7" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -4618,8 +4748,11 @@
         <f>cases!V8/(population_2016!$B8/1000)</f>
         <v>1.9632303319086279</v>
       </c>
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4706,8 +4839,11 @@
         <f>cases!V9/(population_2016!$B9/1000)</f>
         <v>2.5816649104320337</v>
       </c>
+      <c r="W9" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -4794,8 +4930,11 @@
         <f>cases!V10/(population_2016!$B10/1000)</f>
         <v>4.1588986089201203</v>
       </c>
+      <c r="W10" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -4882,8 +5021,11 @@
         <f>cases!V11/(population_2016!$B11/1000)</f>
         <v>1.2406332191950771</v>
       </c>
+      <c r="W11" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4970,8 +5112,11 @@
         <f>cases!V12/(population_2016!$B12/1000)</f>
         <v>2.427566364719369</v>
       </c>
+      <c r="W12" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5058,8 +5203,11 @@
         <f>cases!V13/(population_2016!$B13/1000)</f>
         <v>4.9965518587433158</v>
       </c>
+      <c r="W13" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5146,8 +5294,11 @@
         <f>cases!V14/(population_2016!$B14/1000)</f>
         <v>1.6835931135610709</v>
       </c>
+      <c r="W14" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5234,8 +5385,11 @@
         <f>cases!V15/(population_2016!$B15/1000)</f>
         <v>3.5876021878492033</v>
       </c>
+      <c r="W15" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -5322,8 +5476,11 @@
         <f>cases!V16/(population_2016!$B16/1000)</f>
         <v>2.0779220779220777</v>
       </c>
+      <c r="W16" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5410,8 +5567,11 @@
         <f>cases!V17/(population_2016!$B17/1000)</f>
         <v>6.849965572096778</v>
       </c>
+      <c r="W17" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -5498,8 +5658,11 @@
         <f>cases!V18/(population_2016!$B18/1000)</f>
         <v>1.1881188118811881</v>
       </c>
+      <c r="W18" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>111</v>
       </c>
@@ -5586,8 +5749,11 @@
         <f>cases!V19/(population_2016!$B19/1000)</f>
         <v>3.1071217202604062</v>
       </c>
+      <c r="W19" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -5674,8 +5840,11 @@
         <f>cases!V20/(population_2016!$B20/1000)</f>
         <v>6.7629623444936122</v>
       </c>
+      <c r="W20" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -5762,8 +5931,11 @@
         <f>cases!V21/(population_2016!$B21/1000)</f>
         <v>1.5873703046307921</v>
       </c>
+      <c r="W21" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -5850,8 +6022,11 @@
         <f>cases!V22/(population_2016!$B22/1000)</f>
         <v>3.4903846153846154</v>
       </c>
+      <c r="W22" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -5938,8 +6113,11 @@
         <f>cases!V23/(population_2016!$B23/1000)</f>
         <v>1.2746972594008923</v>
       </c>
+      <c r="W23" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -6026,8 +6204,11 @@
         <f>cases!V24/(population_2016!$B24/1000)</f>
         <v>4.1595233411090193</v>
       </c>
+      <c r="W24" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -6114,8 +6295,11 @@
         <f>cases!V25/(population_2016!$B25/1000)</f>
         <v>2.9944838455476752</v>
       </c>
+      <c r="W25" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -6202,8 +6386,11 @@
         <f>cases!V26/(population_2016!$B26/1000)</f>
         <v>1.008471157724889</v>
       </c>
+      <c r="W26" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -6290,8 +6477,11 @@
         <f>cases!V27/(population_2016!$B27/1000)</f>
         <v>2.7421378556684339</v>
       </c>
+      <c r="W27" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -6378,8 +6568,11 @@
         <f>cases!V28/(population_2016!$B28/1000)</f>
         <v>3.7545495179107333</v>
       </c>
+      <c r="W28" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -6466,8 +6659,11 @@
         <f>cases!V29/(population_2016!$B29/1000)</f>
         <v>2.1715526601520088</v>
       </c>
+      <c r="W29" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -6554,8 +6750,11 @@
         <f>cases!V30/(population_2016!$B30/1000)</f>
         <v>4.4785095520210874</v>
       </c>
+      <c r="W30" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -6642,8 +6841,11 @@
         <f>cases!V31/(population_2016!$B31/1000)</f>
         <v>5.055684756388219</v>
       </c>
+      <c r="W31" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -6730,8 +6932,11 @@
         <f>cases!V32/(population_2016!$B32/1000)</f>
         <v>2.9269933834249184</v>
       </c>
+      <c r="W32" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -6818,8 +7023,11 @@
         <f>cases!V33/(population_2016!$B33/1000)</f>
         <v>3.6773650879717485</v>
       </c>
+      <c r="W33" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -6905,6 +7113,9 @@
       <c r="V34" s="3">
         <f>cases!V34/(population_2016!$B34/1000)</f>
         <v>3.4462386766443478</v>
+      </c>
+      <c r="W34" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -6914,10 +7125,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9609F4-1A5A-459D-8297-63DB4B7007A3}">
-  <dimension ref="A1:AR36"/>
+  <dimension ref="A1:AR37"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AQ40" sqref="AQ40"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12413,6 +12624,142 @@
         <v>36.88680057514199</v>
       </c>
     </row>
+    <row r="37" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="A37" s="19">
+        <v>43940</v>
+      </c>
+      <c r="B37" s="17">
+        <f>mtl_newcases!C38</f>
+        <v>8964</v>
+      </c>
+      <c r="C37" s="17">
+        <f>mtl_newcases!B38</f>
+        <v>507</v>
+      </c>
+      <c r="D37">
+        <v>525</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" t="s">
+        <v>102</v>
+      </c>
+      <c r="H37" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" t="s">
+        <v>102</v>
+      </c>
+      <c r="J37" t="s">
+        <v>102</v>
+      </c>
+      <c r="K37" t="s">
+        <v>102</v>
+      </c>
+      <c r="L37" t="s">
+        <v>102</v>
+      </c>
+      <c r="M37" t="s">
+        <v>102</v>
+      </c>
+      <c r="N37" t="s">
+        <v>102</v>
+      </c>
+      <c r="O37" t="s">
+        <v>102</v>
+      </c>
+      <c r="P37" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>102</v>
+      </c>
+      <c r="R37" t="s">
+        <v>102</v>
+      </c>
+      <c r="S37" t="s">
+        <v>102</v>
+      </c>
+      <c r="T37" t="s">
+        <v>102</v>
+      </c>
+      <c r="U37" t="s">
+        <v>102</v>
+      </c>
+      <c r="V37" t="s">
+        <v>102</v>
+      </c>
+      <c r="W37" t="s">
+        <v>102</v>
+      </c>
+      <c r="X37" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AP37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12420,11 +12767,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B06CD11-991A-4E1F-B148-C34F5A6BF33A}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13541,6 +13888,29 @@
         <v>3555</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>43940</v>
+      </c>
+      <c r="B49">
+        <v>19319</v>
+      </c>
+      <c r="C49">
+        <v>939</v>
+      </c>
+      <c r="D49">
+        <v>1169</v>
+      </c>
+      <c r="E49">
+        <v>198</v>
+      </c>
+      <c r="F49">
+        <v>148482</v>
+      </c>
+      <c r="G49">
+        <v>3847</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13548,10 +13918,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6959A7-678F-4782-AEA8-33A89ACBBFD9}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14203,7 +14573,7 @@
       <c r="A37" s="19">
         <v>43939</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="23">
         <v>13</v>
       </c>
       <c r="C37">
@@ -14218,6 +14588,28 @@
       </c>
       <c r="G37">
         <f t="shared" ref="G37" si="7">C37-F37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="19">
+        <v>43940</v>
+      </c>
+      <c r="B38" s="23">
+        <v>507</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ref="C38" si="8">C37+B38</f>
+        <v>8964</v>
+      </c>
+      <c r="E38" s="19">
+        <v>43940</v>
+      </c>
+      <c r="F38">
+        <v>8964</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38" si="9">C38-F38</f>
         <v>0</v>
       </c>
     </row>
@@ -14231,9 +14623,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E261AEA-18EA-4FE9-ACAC-1FB61BEBD535}">
   <dimension ref="A1:HH81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U2" sqref="U2:U35"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V68" sqref="V68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14308,7 +14700,9 @@
       <c r="U1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="5"/>
+      <c r="V1" s="5" t="s">
+        <v>305</v>
+      </c>
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
@@ -14568,7 +14962,9 @@
       <c r="U2" s="7">
         <v>663</v>
       </c>
-      <c r="V2" s="7"/>
+      <c r="V2" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
@@ -14828,7 +15224,9 @@
       <c r="U3" s="9">
         <v>138</v>
       </c>
-      <c r="V3" s="9"/>
+      <c r="V3" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
       <c r="Y3" s="9"/>
@@ -15088,7 +15486,9 @@
       <c r="U4" s="7">
         <v>5</v>
       </c>
-      <c r="V4" s="7"/>
+      <c r="V4" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
@@ -15348,7 +15748,9 @@
       <c r="U5" s="9">
         <v>15</v>
       </c>
-      <c r="V5" s="9"/>
+      <c r="V5" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
@@ -15608,7 +16010,9 @@
       <c r="U6" s="7">
         <v>839</v>
       </c>
-      <c r="V6" s="7"/>
+      <c r="V6" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
@@ -15868,7 +16272,9 @@
       <c r="U7" s="9">
         <v>300</v>
       </c>
-      <c r="V7" s="9"/>
+      <c r="V7" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
@@ -16128,7 +16534,9 @@
       <c r="U8" s="7">
         <v>96</v>
       </c>
-      <c r="V8" s="7"/>
+      <c r="V8" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
@@ -16388,7 +16796,9 @@
       <c r="U9" s="9">
         <v>49</v>
       </c>
-      <c r="V9" s="9"/>
+      <c r="V9" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
@@ -16648,7 +17058,9 @@
       <c r="U10" s="7">
         <v>29</v>
       </c>
-      <c r="V10" s="7"/>
+      <c r="V10" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
@@ -16908,7 +17320,9 @@
       <c r="U11" s="9">
         <v>25</v>
       </c>
-      <c r="V11" s="9"/>
+      <c r="V11" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
@@ -17168,7 +17582,9 @@
       <c r="U12" s="7">
         <v>108</v>
       </c>
-      <c r="V12" s="7"/>
+      <c r="V12" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
@@ -17428,7 +17844,9 @@
       <c r="U13" s="9">
         <v>384</v>
       </c>
-      <c r="V13" s="9"/>
+      <c r="V13" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W13" s="9"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
@@ -17688,7 +18106,9 @@
       <c r="U14" s="7">
         <v>31</v>
       </c>
-      <c r="V14" s="7"/>
+      <c r="V14" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
@@ -17948,7 +18368,9 @@
       <c r="U15" s="9">
         <v>488</v>
       </c>
-      <c r="V15" s="9"/>
+      <c r="V15" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
@@ -18208,7 +18630,9 @@
       <c r="U16" s="7">
         <v>8</v>
       </c>
-      <c r="V16" s="7"/>
+      <c r="V16" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
       <c r="Y16" s="7"/>
@@ -18468,7 +18892,9 @@
       <c r="U17" s="9">
         <v>577</v>
       </c>
-      <c r="V17" s="9"/>
+      <c r="V17" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W17" s="9"/>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
@@ -18728,7 +19154,9 @@
       <c r="U18" s="7">
         <v>6</v>
       </c>
-      <c r="V18" s="7"/>
+      <c r="V18" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
@@ -18988,7 +19416,9 @@
       <c r="U19" s="9">
         <v>63</v>
       </c>
-      <c r="V19" s="9"/>
+      <c r="V19" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
@@ -19248,7 +19678,9 @@
       <c r="U20" s="7">
         <v>162</v>
       </c>
-      <c r="V20" s="7"/>
+      <c r="V20" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
       <c r="Y20" s="7"/>
@@ -19508,7 +19940,9 @@
       <c r="U21" s="9">
         <v>110</v>
       </c>
-      <c r="V21" s="9"/>
+      <c r="V21" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
@@ -19768,7 +20202,9 @@
       <c r="U22" s="7">
         <v>363</v>
       </c>
-      <c r="V22" s="7"/>
+      <c r="V22" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
       <c r="Y22" s="7"/>
@@ -20028,7 +20464,9 @@
       <c r="U23" s="9">
         <v>40</v>
       </c>
-      <c r="V23" s="9"/>
+      <c r="V23" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W23" s="9"/>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
@@ -20288,7 +20726,9 @@
       <c r="U24" s="7">
         <v>444</v>
       </c>
-      <c r="V24" s="7"/>
+      <c r="V24" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
@@ -20548,7 +20988,9 @@
       <c r="U25" s="9">
         <v>418</v>
       </c>
-      <c r="V25" s="9"/>
+      <c r="V25" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
@@ -20808,7 +21250,9 @@
       <c r="U26" s="7">
         <v>5</v>
       </c>
-      <c r="V26" s="7"/>
+      <c r="V26" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -21068,7 +21512,9 @@
       <c r="U27" s="9">
         <v>271</v>
       </c>
-      <c r="V27" s="9"/>
+      <c r="V27" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
       <c r="Y27" s="9"/>
@@ -21328,7 +21774,9 @@
       <c r="U28" s="7">
         <v>294</v>
       </c>
-      <c r="V28" s="7"/>
+      <c r="V28" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
@@ -21588,7 +22036,9 @@
       <c r="U29" s="20">
         <v>2</v>
       </c>
-      <c r="V29" s="22"/>
+      <c r="V29" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W29" s="22"/>
       <c r="X29" s="22"/>
       <c r="Y29" s="22"/>
@@ -21848,7 +22298,9 @@
       <c r="U30" s="7">
         <v>350</v>
       </c>
-      <c r="V30" s="7"/>
+      <c r="V30" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
@@ -22108,7 +22560,9 @@
       <c r="U31" s="9">
         <v>350</v>
       </c>
-      <c r="V31" s="9"/>
+      <c r="V31" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
       <c r="Y31" s="9"/>
@@ -22368,7 +22822,9 @@
       <c r="U32" s="7">
         <v>261</v>
       </c>
-      <c r="V32" s="7"/>
+      <c r="V32" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
@@ -22628,7 +23084,9 @@
       <c r="U33" s="9">
         <v>529</v>
       </c>
-      <c r="V33" s="9"/>
+      <c r="V33" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W33" s="9"/>
       <c r="X33" s="9"/>
       <c r="Y33" s="9"/>
@@ -22888,7 +23346,9 @@
       <c r="U34" s="7">
         <v>70</v>
       </c>
-      <c r="V34" s="7"/>
+      <c r="V34" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W34" s="7"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="7"/>
@@ -23148,7 +23608,9 @@
       <c r="U35" s="9">
         <v>964</v>
       </c>
-      <c r="V35" s="9"/>
+      <c r="V35" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W35" s="9"/>
       <c r="X35" s="9"/>
       <c r="Y35" s="9"/>
@@ -23408,7 +23870,9 @@
       <c r="U36" s="11">
         <v>8457</v>
       </c>
-      <c r="V36" s="11"/>
+      <c r="V36" s="11">
+        <v>8964</v>
+      </c>
       <c r="W36" s="11"/>
       <c r="X36" s="11"/>
       <c r="Y36" s="11"/>
@@ -27603,7 +28067,9 @@
       <c r="U56" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="V56" s="5"/>
+      <c r="V56" s="5" t="s">
+        <v>305</v>
+      </c>
       <c r="W56" s="5"/>
       <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
@@ -27861,7 +28327,9 @@
       <c r="U57" s="7">
         <v>46</v>
       </c>
-      <c r="V57" s="7"/>
+      <c r="V57" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W57" s="7"/>
       <c r="X57" s="7"/>
       <c r="Y57" s="7"/>
@@ -28119,7 +28587,9 @@
       <c r="U58" s="9">
         <v>35</v>
       </c>
-      <c r="V58" s="9"/>
+      <c r="V58" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W58" s="9"/>
       <c r="X58" s="9"/>
       <c r="Y58" s="9"/>
@@ -28377,7 +28847,9 @@
       <c r="U59" s="7">
         <v>197</v>
       </c>
-      <c r="V59" s="7"/>
+      <c r="V59" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W59" s="7"/>
       <c r="X59" s="7"/>
       <c r="Y59" s="7"/>
@@ -28635,7 +29107,9 @@
       <c r="U60" s="9">
         <v>1022</v>
       </c>
-      <c r="V60" s="9"/>
+      <c r="V60" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W60" s="9"/>
       <c r="X60" s="9"/>
       <c r="Y60" s="9"/>
@@ -28893,7 +29367,9 @@
       <c r="U61" s="7">
         <v>1250</v>
       </c>
-      <c r="V61" s="7"/>
+      <c r="V61" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W61" s="7"/>
       <c r="X61" s="7"/>
       <c r="Y61" s="7"/>
@@ -29151,7 +29627,9 @@
       <c r="U62" s="9">
         <v>1451</v>
       </c>
-      <c r="V62" s="9"/>
+      <c r="V62" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W62" s="9"/>
       <c r="X62" s="9"/>
       <c r="Y62" s="9"/>
@@ -29409,7 +29887,9 @@
       <c r="U63" s="7">
         <v>1247</v>
       </c>
-      <c r="V63" s="7"/>
+      <c r="V63" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W63" s="7"/>
       <c r="X63" s="7"/>
       <c r="Y63" s="7"/>
@@ -29667,7 +30147,9 @@
       <c r="U64" s="9">
         <v>802</v>
       </c>
-      <c r="V64" s="9"/>
+      <c r="V64" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W64" s="9"/>
       <c r="X64" s="9"/>
       <c r="Y64" s="9"/>
@@ -29925,7 +30407,9 @@
       <c r="U65" s="7">
         <v>695</v>
       </c>
-      <c r="V65" s="7"/>
+      <c r="V65" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W65" s="7"/>
       <c r="X65" s="7"/>
       <c r="Y65" s="7"/>
@@ -30183,7 +30667,9 @@
       <c r="U66" s="9">
         <v>1689</v>
       </c>
-      <c r="V66" s="9"/>
+      <c r="V66" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="W66" s="9"/>
       <c r="X66" s="9"/>
       <c r="Y66" s="9"/>
@@ -30441,7 +30927,9 @@
       <c r="U67" s="7">
         <v>23</v>
       </c>
-      <c r="V67" s="7"/>
+      <c r="V67" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="W67" s="7"/>
       <c r="X67" s="7"/>
       <c r="Y67" s="7"/>
@@ -30699,7 +31187,9 @@
       <c r="U68" s="15">
         <v>8457</v>
       </c>
-      <c r="V68" s="15"/>
+      <c r="V68" s="15">
+        <v>8964</v>
+      </c>
       <c r="W68" s="15"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
@@ -30959,6 +31449,9 @@
       <c r="U70">
         <v>513</v>
       </c>
+      <c r="V70">
+        <v>525</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">

</xml_diff>

<commit_message>
Update data (2020-04-28 v2)
Santé Montréal posted updated data.
</commit_message>
<xml_diff>
--- a/data/covid19_MTL.xlsx
+++ b/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07AAD66-A7BF-46C2-A73E-9939961DF74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA69E49F-5F36-41B8-B552-374011A92FC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15940" yWindow="4800" windowWidth="24450" windowHeight="15170" tabRatio="512" activeTab="3" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="12630" yWindow="5290" windowWidth="24450" windowHeight="15170" tabRatio="512" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1528,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5D96B4-0147-4A32-9FAF-C932A9839F40}">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="X37" sqref="X37"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="AE36" sqref="AE36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4861,7 +4861,7 @@
         <v>604</v>
       </c>
       <c r="AE35">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
   </sheetData>
@@ -4875,7 +4875,7 @@
   <dimension ref="A1:AE34"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
@@ -9073,7 +9073,7 @@
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP48" sqref="AP48"/>
+      <selection pane="topRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16032,18 +16032,18 @@
       </c>
       <c r="B45" s="17">
         <f>mtl_newcases!C46</f>
-        <v>12486</v>
+        <v>12487</v>
       </c>
       <c r="C45" s="17">
         <f>mtl_newcases!B46</f>
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D45">
-        <v>983</v>
+        <v>1039</v>
       </c>
       <c r="E45">
         <f t="shared" ref="E45" si="416">D45-D44</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="F45" cm="1">
         <f t="array" ref="F45:O45">TRANSPOSE(santemontreal!AD$57:AD$66)</f>
@@ -16206,7 +16206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B06CD11-991A-4E1F-B148-C34F5A6BF33A}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
     </sheetView>
@@ -18394,7 +18394,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19245,17 +19245,17 @@
         <v>43948</v>
       </c>
       <c r="B46" s="24">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C46">
         <f t="shared" si="13"/>
-        <v>12486</v>
+        <v>12487</v>
       </c>
       <c r="E46" s="19">
         <v>43948</v>
       </c>
       <c r="F46">
-        <v>12486</v>
+        <v>12487</v>
       </c>
       <c r="G46">
         <f>C46-F46</f>
@@ -19272,9 +19272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E261AEA-18EA-4FE9-ACAC-1FB61BEBD535}">
   <dimension ref="A1:HH81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD35" sqref="AD2:AD35"/>
+      <selection pane="topRight" activeCell="AD69" sqref="AD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28826,7 +28826,7 @@
         <v>604</v>
       </c>
       <c r="AD35" s="9">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="AE35" s="9"/>
       <c r="AF35" s="9"/>
@@ -29104,7 +29104,7 @@
         <v>12034</v>
       </c>
       <c r="AD36" s="11">
-        <v>12486</v>
+        <v>12487</v>
       </c>
       <c r="AE36" s="11"/>
       <c r="AF36" s="11"/>
@@ -36353,7 +36353,7 @@
         <v>65</v>
       </c>
       <c r="AD67" s="7">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AE67" s="7"/>
       <c r="AF67" s="7"/>
@@ -36629,7 +36629,7 @@
         <v>12034</v>
       </c>
       <c r="AD68" s="15">
-        <v>12486</v>
+        <v>12487</v>
       </c>
       <c r="AE68" s="15"/>
       <c r="AF68" s="15"/>
@@ -36907,7 +36907,7 @@
         <v>983</v>
       </c>
       <c r="AD70">
-        <v>983</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add missing data point
Fill in missing Montreal deaths data point using data from: https://web.archive.org/web/20200430154124/https://www.quebec.ca/sante/problemes-de-sante/a-z/coronavirus-2019/situation-coronavirus-quebec/
</commit_message>
<xml_diff>
--- a/data/covid19_MTL.xlsx
+++ b/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA899EB7-270A-4053-B52A-FA981E04D674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C131ACF-13B7-4FDC-9D72-6E08D234C4FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="3690" windowWidth="31460" windowHeight="15170" tabRatio="512" activeTab="5" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="6840" yWindow="3690" windowWidth="31460" windowHeight="15170" tabRatio="512" activeTab="2" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="315">
   <si>
     <t>borough</t>
   </si>
@@ -9491,9 +9491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9609F4-1A5A-459D-8297-63DB4B7007A3}">
   <dimension ref="A1:AS47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D46" sqref="D46"/>
+      <selection pane="topRight" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16628,11 +16628,12 @@
         <f t="shared" ref="C46:C47" si="438">B46-B45</f>
         <v>324</v>
       </c>
-      <c r="D46" t="s">
-        <v>102</v>
-      </c>
-      <c r="E46" t="s">
-        <v>102</v>
+      <c r="D46">
+        <v>1078</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="417"/>
+        <v>39</v>
       </c>
       <c r="F46" t="s">
         <v>102</v>
@@ -16769,8 +16770,9 @@
       <c r="D47">
         <v>1146</v>
       </c>
-      <c r="E47" t="s">
-        <v>102</v>
+      <c r="E47">
+        <f t="shared" si="417"/>
+        <v>68</v>
       </c>
       <c r="F47" t="s">
         <v>102</v>
@@ -17035,7 +17037,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C58" si="0">B4-B3</f>
+        <f t="shared" ref="C4:C57" si="0">B4-B3</f>
         <v>1</v>
       </c>
       <c r="D4">
@@ -20044,7 +20046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E261AEA-18EA-4FE9-ACAC-1FB61BEBD535}">
   <dimension ref="A1:HH81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AF56" sqref="AF56"/>
     </sheetView>

</xml_diff>

<commit_message>
Updata data (2020-05-01 v2)
Santé Montréal posted the remaining missing data for the day (cases per borough/city and by age group).
</commit_message>
<xml_diff>
--- a/data/covid19_MTL.xlsx
+++ b/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AFAF5D-0BFE-4048-9D61-3806EEEF8888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F2A31A-2265-4EC7-9F78-CB72D8B17721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="4270" windowWidth="23520" windowHeight="15660" tabRatio="512" activeTab="5" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="7900" yWindow="4700" windowWidth="30500" windowHeight="15660" tabRatio="512" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="320">
   <si>
     <t>borough</t>
   </si>
@@ -916,9 +916,6 @@
     <t>25AVRIL, 05h05</t>
   </si>
   <si>
-    <t>9,1</t>
-  </si>
-  <si>
     <t>new_cases_qc</t>
   </si>
   <si>
@@ -943,76 +940,10 @@
     <t>0,9</t>
   </si>
   <si>
-    <t>3,3</t>
-  </si>
-  <si>
-    <t>9,0</t>
-  </si>
-  <si>
     <t>26AVRIL, 18h30</t>
   </si>
   <si>
-    <t>604,4</t>
-  </si>
-  <si>
     <t>27AVRIL, 18h30</t>
-  </si>
-  <si>
-    <t>TOTAL DE CAS CONFIRMÉS¹</t>
-  </si>
-  <si>
-    <t>RÉPARTITION DES CAS (%)</t>
-  </si>
-  <si>
-    <t>TAUX POUR</t>
-  </si>
-  <si>
-    <t>100 000</t>
-  </si>
-  <si>
-    <t>PERSONNES</t>
-  </si>
-  <si>
-    <t>102,8</t>
-  </si>
-  <si>
-    <t>101,0</t>
-  </si>
-  <si>
-    <t>204,6</t>
-  </si>
-  <si>
-    <t>11,4</t>
-  </si>
-  <si>
-    <t>438,4</t>
-  </si>
-  <si>
-    <t>13,1</t>
-  </si>
-  <si>
-    <t>495,8</t>
-  </si>
-  <si>
-    <t>15,1</t>
-  </si>
-  <si>
-    <t>675,4</t>
-  </si>
-  <si>
-    <t>634,7</t>
-  </si>
-  <si>
-    <t>513,9</t>
-  </si>
-  <si>
-    <t>780,9</t>
-  </si>
-  <si>
-    <t>24,1</t>
-  </si>
-  <si>
-    <t>2 966,1</t>
   </si>
   <si>
     <t>28 AVRIL, 18h30</t>
@@ -1022,6 +953,87 @@
   </si>
   <si>
     <t>30 AVRIL, 18h30</t>
+  </si>
+  <si>
+    <t>n.p.</t>
+  </si>
+  <si>
+    <t>&lt; 5</t>
+  </si>
+  <si>
+    <t>676,7</t>
+  </si>
+  <si>
+    <t>1 245</t>
+  </si>
+  <si>
+    <t>60,3</t>
+  </si>
+  <si>
+    <t>111,1</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>219,2</t>
+  </si>
+  <si>
+    <t>11,2</t>
+  </si>
+  <si>
+    <t>482,1</t>
+  </si>
+  <si>
+    <t>12,7</t>
+  </si>
+  <si>
+    <t>539,7</t>
+  </si>
+  <si>
+    <t>14,7</t>
+  </si>
+  <si>
+    <t>734,7</t>
+  </si>
+  <si>
+    <t>* 3,6</t>
+  </si>
+  <si>
+    <t>12,9</t>
+  </si>
+  <si>
+    <t>699,7</t>
+  </si>
+  <si>
+    <t>* 9,0</t>
+  </si>
+  <si>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>573,0</t>
+  </si>
+  <si>
+    <t>40,2</t>
+  </si>
+  <si>
+    <t>9,3</t>
+  </si>
+  <si>
+    <t>898,4</t>
+  </si>
+  <si>
+    <t>140,3</t>
+  </si>
+  <si>
+    <t>25,3</t>
+  </si>
+  <si>
+    <t>3 479,8</t>
+  </si>
+  <si>
+    <t>908,5</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1220,7 +1232,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1537,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5D96B4-0147-4A32-9FAF-C932A9839F40}">
   <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AH35"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="AH35" sqref="AH2:AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1752,8 +1763,8 @@
       <c r="AG2" t="s">
         <v>102</v>
       </c>
-      <c r="AH2" t="s">
-        <v>102</v>
+      <c r="AH2">
+        <v>1185</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
@@ -1856,8 +1867,8 @@
       <c r="AG3" t="s">
         <v>102</v>
       </c>
-      <c r="AH3" t="s">
-        <v>102</v>
+      <c r="AH3">
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.35">
@@ -1960,8 +1971,8 @@
       <c r="AG4" t="s">
         <v>102</v>
       </c>
-      <c r="AH4" t="s">
-        <v>102</v>
+      <c r="AH4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
@@ -2064,8 +2075,8 @@
       <c r="AG5" t="s">
         <v>102</v>
       </c>
-      <c r="AH5" t="s">
-        <v>102</v>
+      <c r="AH5">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.35">
@@ -2168,8 +2179,8 @@
       <c r="AG6" t="s">
         <v>102</v>
       </c>
-      <c r="AH6" t="s">
-        <v>102</v>
+      <c r="AH6">
+        <v>1225</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
@@ -2272,8 +2283,8 @@
       <c r="AG7" t="s">
         <v>102</v>
       </c>
-      <c r="AH7" t="s">
-        <v>102</v>
+      <c r="AH7">
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
@@ -2376,8 +2387,8 @@
       <c r="AG8" t="s">
         <v>102</v>
       </c>
-      <c r="AH8" t="s">
-        <v>102</v>
+      <c r="AH8">
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
@@ -2480,8 +2491,8 @@
       <c r="AG9" t="s">
         <v>102</v>
       </c>
-      <c r="AH9" t="s">
-        <v>102</v>
+      <c r="AH9">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
@@ -2584,8 +2595,8 @@
       <c r="AG10" t="s">
         <v>102</v>
       </c>
-      <c r="AH10" t="s">
-        <v>102</v>
+      <c r="AH10">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
@@ -2688,8 +2699,8 @@
       <c r="AG11" t="s">
         <v>102</v>
       </c>
-      <c r="AH11" t="s">
-        <v>102</v>
+      <c r="AH11">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
@@ -2792,8 +2803,8 @@
       <c r="AG12" t="s">
         <v>102</v>
       </c>
-      <c r="AH12" t="s">
-        <v>102</v>
+      <c r="AH12">
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.35">
@@ -2896,8 +2907,8 @@
       <c r="AG13" t="s">
         <v>102</v>
       </c>
-      <c r="AH13" t="s">
-        <v>102</v>
+      <c r="AH13">
+        <v>561</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.35">
@@ -3000,8 +3011,8 @@
       <c r="AG14" t="s">
         <v>102</v>
       </c>
-      <c r="AH14" t="s">
-        <v>102</v>
+      <c r="AH14">
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.35">
@@ -3104,8 +3115,8 @@
       <c r="AG15" t="s">
         <v>102</v>
       </c>
-      <c r="AH15" t="s">
-        <v>102</v>
+      <c r="AH15">
+        <v>1014</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.35">
@@ -3208,8 +3219,8 @@
       <c r="AG16" t="s">
         <v>102</v>
       </c>
-      <c r="AH16" t="s">
-        <v>102</v>
+      <c r="AH16">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.35">
@@ -3312,8 +3323,8 @@
       <c r="AG17" t="s">
         <v>102</v>
       </c>
-      <c r="AH17" t="s">
-        <v>102</v>
+      <c r="AH17">
+        <v>1316</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.35">
@@ -3416,8 +3427,8 @@
       <c r="AG18" t="s">
         <v>102</v>
       </c>
-      <c r="AH18" t="s">
-        <v>102</v>
+      <c r="AH18">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.35">
@@ -3520,8 +3531,8 @@
       <c r="AG19" t="s">
         <v>102</v>
       </c>
-      <c r="AH19" t="s">
-        <v>102</v>
+      <c r="AH19">
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.35">
@@ -3624,8 +3635,8 @@
       <c r="AG20" t="s">
         <v>102</v>
       </c>
-      <c r="AH20" t="s">
-        <v>102</v>
+      <c r="AH20">
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.35">
@@ -3728,8 +3739,8 @@
       <c r="AG21" t="s">
         <v>102</v>
       </c>
-      <c r="AH21" t="s">
-        <v>102</v>
+      <c r="AH21">
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.35">
@@ -3832,8 +3843,8 @@
       <c r="AG22" t="s">
         <v>102</v>
       </c>
-      <c r="AH22" t="s">
-        <v>102</v>
+      <c r="AH22">
+        <v>566</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.35">
@@ -3936,8 +3947,8 @@
       <c r="AG23" t="s">
         <v>102</v>
       </c>
-      <c r="AH23" t="s">
-        <v>102</v>
+      <c r="AH23">
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.35">
@@ -4040,8 +4051,8 @@
       <c r="AG24" t="s">
         <v>102</v>
       </c>
-      <c r="AH24" t="s">
-        <v>102</v>
+      <c r="AH24">
+        <v>1029</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.35">
@@ -4144,8 +4155,8 @@
       <c r="AG25" t="s">
         <v>102</v>
       </c>
-      <c r="AH25" t="s">
-        <v>102</v>
+      <c r="AH25">
+        <v>777</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.35">
@@ -4248,8 +4259,8 @@
       <c r="AG26" t="s">
         <v>102</v>
       </c>
-      <c r="AH26" t="s">
-        <v>102</v>
+      <c r="AH26">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.35">
@@ -4352,8 +4363,8 @@
       <c r="AG27" t="s">
         <v>102</v>
       </c>
-      <c r="AH27" t="s">
-        <v>102</v>
+      <c r="AH27">
+        <v>518</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.35">
@@ -4456,8 +4467,8 @@
       <c r="AG28" t="s">
         <v>102</v>
       </c>
-      <c r="AH28" t="s">
-        <v>102</v>
+      <c r="AH28">
+        <v>582</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.35">
@@ -4560,8 +4571,8 @@
       <c r="AG29" t="s">
         <v>102</v>
       </c>
-      <c r="AH29" t="s">
-        <v>102</v>
+      <c r="AH29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.35">
@@ -4664,8 +4675,8 @@
       <c r="AG30" t="s">
         <v>102</v>
       </c>
-      <c r="AH30" t="s">
-        <v>102</v>
+      <c r="AH30">
+        <v>563</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.35">
@@ -4768,8 +4779,8 @@
       <c r="AG31" t="s">
         <v>102</v>
       </c>
-      <c r="AH31" t="s">
-        <v>102</v>
+      <c r="AH31">
+        <v>620</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.35">
@@ -4872,8 +4883,8 @@
       <c r="AG32" t="s">
         <v>102</v>
       </c>
-      <c r="AH32" t="s">
-        <v>102</v>
+      <c r="AH32">
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.35">
@@ -4976,8 +4987,8 @@
       <c r="AG33" t="s">
         <v>102</v>
       </c>
-      <c r="AH33" t="s">
-        <v>102</v>
+      <c r="AH33">
+        <v>998</v>
       </c>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.35">
@@ -5080,8 +5091,8 @@
       <c r="AG34" t="s">
         <v>102</v>
       </c>
-      <c r="AH34" t="s">
-        <v>102</v>
+      <c r="AH34">
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.35">
@@ -5184,8 +5195,8 @@
       <c r="AG35" t="s">
         <v>102</v>
       </c>
-      <c r="AH35" t="s">
-        <v>102</v>
+      <c r="AH35">
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -5199,8 +5210,8 @@
   <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG1" sqref="AG1:AH34"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5464,8 +5475,9 @@
       <c r="AG2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH2" s="3" t="s">
-        <v>102</v>
+      <c r="AH2" s="3">
+        <f>cases!AH2/(population_2016!$B2/1000)</f>
+        <v>8.8271444001638795</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
@@ -5596,8 +5608,9 @@
       <c r="AG3" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH3" s="3" t="s">
-        <v>102</v>
+      <c r="AH3" s="3">
+        <f>cases!AH3/(population_2016!$B3/1000)</f>
+        <v>7.5708010094401343</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.35">
@@ -5728,8 +5741,9 @@
       <c r="AG4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH4" s="3" t="s">
-        <v>102</v>
+      <c r="AH4" s="3">
+        <f>cases!AH4/(population_2016!$B4/1000)</f>
+        <v>1.5694480774261053</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
@@ -5860,8 +5874,9 @@
       <c r="AG5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH5" s="3" t="s">
-        <v>102</v>
+      <c r="AH5" s="3">
+        <f>cases!AH5/(population_2016!$B5/1000)</f>
+        <v>1.3972262471537982</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.35">
@@ -5992,8 +6007,9 @@
       <c r="AG6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH6" s="3" t="s">
-        <v>102</v>
+      <c r="AH6" s="3">
+        <f>cases!AH6/(population_2016!$B6/1000)</f>
+        <v>7.3564736968532305</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
@@ -6124,8 +6140,9 @@
       <c r="AG7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH7" s="3" t="s">
-        <v>102</v>
+      <c r="AH7" s="3">
+        <f>cases!AH7/(population_2016!$B7/1000)</f>
+        <v>10.909763313609467</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
@@ -6256,8 +6273,9 @@
       <c r="AG8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH8" s="3" t="s">
-        <v>102</v>
+      <c r="AH8" s="3">
+        <f>cases!AH8/(population_2016!$B8/1000)</f>
+        <v>3.7628581361582034</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
@@ -6388,8 +6406,9 @@
       <c r="AG9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH9" s="3" t="s">
-        <v>102</v>
+      <c r="AH9" s="3">
+        <f>cases!AH9/(population_2016!$B9/1000)</f>
+        <v>5.0052687038988406</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
@@ -6520,8 +6539,9 @@
       <c r="AG10" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH10" s="3" t="s">
-        <v>102</v>
+      <c r="AH10" s="3">
+        <f>cases!AH10/(population_2016!$B10/1000)</f>
+        <v>5.4495912806539515</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
@@ -6652,8 +6672,9 @@
       <c r="AG11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH11" s="3" t="s">
-        <v>102</v>
+      <c r="AH11" s="3">
+        <f>cases!AH11/(population_2016!$B11/1000)</f>
+        <v>2.5805170959257606</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
@@ -6784,8 +6805,9 @@
       <c r="AG12" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH12" s="3" t="s">
-        <v>102</v>
+      <c r="AH12" s="3">
+        <f>cases!AH12/(population_2016!$B12/1000)</f>
+        <v>4.1808087392389135</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.35">
@@ -6916,8 +6938,9 @@
       <c r="AG13" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH13" s="3" t="s">
-        <v>102</v>
+      <c r="AH13" s="3">
+        <f>cases!AH13/(population_2016!$B13/1000)</f>
+        <v>7.2996499811328128</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.35">
@@ -7048,8 +7071,9 @@
       <c r="AG14" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH14" s="3" t="s">
-        <v>102</v>
+      <c r="AH14" s="3">
+        <f>cases!AH14/(population_2016!$B14/1000)</f>
+        <v>4.1275186009884317</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.35">
@@ -7180,8 +7204,9 @@
       <c r="AG15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH15" s="3" t="s">
-        <v>102</v>
+      <c r="AH15" s="3">
+        <f>cases!AH15/(population_2016!$B15/1000)</f>
+        <v>7.45456684114568</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.35">
@@ -7312,8 +7337,9 @@
       <c r="AG16" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH16" s="3" t="s">
-        <v>102</v>
+      <c r="AH16" s="3">
+        <f>cases!AH16/(population_2016!$B16/1000)</f>
+        <v>4.6753246753246751</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.35">
@@ -7444,8 +7470,9 @@
       <c r="AG17" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH17" s="3" t="s">
-        <v>102</v>
+      <c r="AH17" s="3">
+        <f>cases!AH17/(population_2016!$B17/1000)</f>
+        <v>15.623145048317783</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.35">
@@ -7576,8 +7603,9 @@
       <c r="AG18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH18" s="3" t="s">
-        <v>102</v>
+      <c r="AH18" s="3">
+        <f>cases!AH18/(population_2016!$B18/1000)</f>
+        <v>2.1782178217821784</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.35">
@@ -7708,8 +7736,9 @@
       <c r="AG19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH19" s="3" t="s">
-        <v>102</v>
+      <c r="AH19" s="3">
+        <f>cases!AH19/(population_2016!$B19/1000)</f>
+        <v>6.1649240481357266</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.35">
@@ -7840,8 +7869,9 @@
       <c r="AG20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH20" s="3" t="s">
-        <v>102</v>
+      <c r="AH20" s="3">
+        <f>cases!AH20/(population_2016!$B20/1000)</f>
+        <v>8.0988561409367961</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.35">
@@ -7972,8 +8002,9 @@
       <c r="AG21" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH21" s="3" t="s">
-        <v>102</v>
+      <c r="AH21" s="3">
+        <f>cases!AH21/(population_2016!$B21/1000)</f>
+        <v>2.7706827135373828</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.35">
@@ -8104,8 +8135,9 @@
       <c r="AG22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH22" s="3" t="s">
-        <v>102</v>
+      <c r="AH22" s="3">
+        <f>cases!AH22/(population_2016!$B22/1000)</f>
+        <v>5.4423076923076925</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.35">
@@ -8236,8 +8268,9 @@
       <c r="AG23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH23" s="3" t="s">
-        <v>102</v>
+      <c r="AH23" s="3">
+        <f>cases!AH23/(population_2016!$B23/1000)</f>
+        <v>2.6449968132568515</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.35">
@@ -8368,8 +8401,9 @@
       <c r="AG24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH24" s="3" t="s">
-        <v>102</v>
+      <c r="AH24" s="3">
+        <f>cases!AH24/(population_2016!$B24/1000)</f>
+        <v>9.6399763918945514</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.35">
@@ -8500,8 +8534,9 @@
       <c r="AG25" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH25" s="3" t="s">
-        <v>102</v>
+      <c r="AH25" s="3">
+        <f>cases!AH25/(population_2016!$B25/1000)</f>
+        <v>5.566301310982162</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.35">
@@ -8632,8 +8667,9 @@
       <c r="AG26" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH26" s="3" t="s">
-        <v>102</v>
+      <c r="AH26" s="3">
+        <f>cases!AH26/(population_2016!$B26/1000)</f>
+        <v>2.0169423154497781</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.35">
@@ -8764,8 +8800,9 @@
       <c r="AG27" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH27" s="3" t="s">
-        <v>102</v>
+      <c r="AH27" s="3">
+        <f>cases!AH27/(population_2016!$B27/1000)</f>
+        <v>5.2414295543773015</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.35">
@@ -8896,8 +8933,9 @@
       <c r="AG28" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH28" s="3" t="s">
-        <v>102</v>
+      <c r="AH28" s="3">
+        <f>cases!AH28/(population_2016!$B28/1000)</f>
+        <v>7.4324755762722683</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.35">
@@ -9028,8 +9066,9 @@
       <c r="AG29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH29" s="3" t="s">
-        <v>102</v>
+      <c r="AH29" s="3">
+        <f>cases!AH29/(population_2016!$B29/1000)</f>
+        <v>2.1715526601520088</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.35">
@@ -9160,8 +9199,9 @@
       <c r="AG30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH30" s="3" t="s">
-        <v>102</v>
+      <c r="AH30" s="3">
+        <f>cases!AH30/(population_2016!$B30/1000)</f>
+        <v>7.2040025079653498</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.35">
@@ -9292,8 +9332,9 @@
       <c r="AG31" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH31" s="3" t="s">
-        <v>102</v>
+      <c r="AH31" s="3">
+        <f>cases!AH31/(population_2016!$B31/1000)</f>
+        <v>8.955784425601987</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.35">
@@ -9424,8 +9465,9 @@
       <c r="AG32" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH32" s="3" t="s">
-        <v>102</v>
+      <c r="AH32" s="3">
+        <f>cases!AH32/(population_2016!$B32/1000)</f>
+        <v>3.9587305147471121</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.35">
@@ -9556,8 +9598,9 @@
       <c r="AG33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH33" s="3" t="s">
-        <v>102</v>
+      <c r="AH33" s="3">
+        <f>cases!AH33/(population_2016!$B33/1000)</f>
+        <v>6.9376377274022785</v>
       </c>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.35">
@@ -9688,8 +9731,9 @@
       <c r="AG34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH34" s="3" t="s">
-        <v>102</v>
+      <c r="AH34" s="3">
+        <f>cases!AH34/(population_2016!$B34/1000)</f>
+        <v>5.5632138637258759</v>
       </c>
     </row>
   </sheetData>
@@ -9701,7 +9745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9609F4-1A5A-459D-8297-63DB4B7007A3}">
   <dimension ref="A1:AS48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E50" sqref="E50"/>
     </sheetView>
@@ -9730,7 +9774,7 @@
         <v>232</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>145</v>
@@ -10971,11 +11015,11 @@
       </c>
       <c r="B10" s="17">
         <f>mtl_newcases!C11</f>
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C10" s="17">
         <f t="shared" si="0"/>
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>102</v>
@@ -11110,11 +11154,11 @@
       </c>
       <c r="B11" s="17">
         <f>mtl_newcases!C12</f>
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C11" s="17">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>102</v>
@@ -11249,11 +11293,11 @@
       </c>
       <c r="B12" s="17">
         <f>mtl_newcases!C13</f>
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="C12" s="17">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>102</v>
@@ -11388,7 +11432,7 @@
       </c>
       <c r="B13" s="17">
         <f>mtl_newcases!C14</f>
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="C13" s="17">
         <f t="shared" si="0"/>
@@ -11527,11 +11571,11 @@
       </c>
       <c r="B14" s="17">
         <f>mtl_newcases!C15</f>
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="C14" s="17">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>102</v>
@@ -11666,11 +11710,11 @@
       </c>
       <c r="B15" s="17">
         <f>mtl_newcases!C16</f>
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C15" s="17">
         <f t="shared" si="0"/>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>102</v>
@@ -11805,11 +11849,11 @@
       </c>
       <c r="B16" s="17">
         <f>mtl_newcases!C17</f>
-        <v>1652</v>
+        <v>1649</v>
       </c>
       <c r="C16" s="17">
         <f t="shared" si="0"/>
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>102</v>
@@ -11948,7 +11992,7 @@
       </c>
       <c r="C17" s="17">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>102</v>
@@ -12253,11 +12297,11 @@
       </c>
       <c r="B19" s="17">
         <f>mtl_newcases!C20</f>
-        <v>2560</v>
+        <v>2561</v>
       </c>
       <c r="C19" s="17">
         <f t="shared" si="0"/>
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>102</v>
@@ -12423,11 +12467,11 @@
       </c>
       <c r="B20" s="17">
         <f>mtl_newcases!C21</f>
-        <v>2956</v>
+        <v>2952</v>
       </c>
       <c r="C20" s="17">
         <f t="shared" si="0"/>
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>102</v>
@@ -12593,11 +12637,11 @@
       </c>
       <c r="B21" s="17">
         <f>mtl_newcases!C22</f>
-        <v>3303</v>
+        <v>3298</v>
       </c>
       <c r="C21" s="17">
         <f t="shared" si="0"/>
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>102</v>
@@ -12763,11 +12807,11 @@
       </c>
       <c r="B22" s="17">
         <f>mtl_newcases!C23</f>
-        <v>3643</v>
+        <v>3639</v>
       </c>
       <c r="C22" s="17">
         <f t="shared" si="0"/>
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>102</v>
@@ -12933,11 +12977,11 @@
       </c>
       <c r="B23" s="17">
         <f>mtl_newcases!C24</f>
-        <v>3892</v>
+        <v>3890</v>
       </c>
       <c r="C23" s="17">
         <f t="shared" si="0"/>
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>102</v>
@@ -13103,7 +13147,7 @@
       </c>
       <c r="B24" s="17">
         <f>mtl_newcases!C25</f>
-        <v>4331</v>
+        <v>4329</v>
       </c>
       <c r="C24" s="17">
         <f t="shared" si="0"/>
@@ -13273,11 +13317,11 @@
       </c>
       <c r="B25" s="17">
         <f>mtl_newcases!C26</f>
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="C25" s="17">
         <f t="shared" si="0"/>
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D25">
         <v>74</v>
@@ -13444,11 +13488,11 @@
       </c>
       <c r="B26" s="17">
         <f>mtl_newcases!C27</f>
-        <v>5082</v>
+        <v>5080</v>
       </c>
       <c r="C26" s="17">
         <f t="shared" si="0"/>
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D26">
         <v>91</v>
@@ -13615,11 +13659,11 @@
       </c>
       <c r="B27" s="17">
         <f>mtl_newcases!C28</f>
-        <v>5406</v>
+        <v>5402</v>
       </c>
       <c r="C27" s="17">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D27">
         <v>100</v>
@@ -13786,11 +13830,11 @@
       </c>
       <c r="B28" s="17">
         <f>mtl_newcases!C29</f>
-        <v>5685</v>
+        <v>5680</v>
       </c>
       <c r="C28" s="17">
         <f t="shared" si="0"/>
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28">
         <v>135</v>
@@ -13957,7 +14001,7 @@
       </c>
       <c r="B29" s="17">
         <f>mtl_newcases!C30</f>
-        <v>5901</v>
+        <v>5896</v>
       </c>
       <c r="C29" s="17">
         <f t="shared" si="0"/>
@@ -14128,11 +14172,11 @@
       </c>
       <c r="B30" s="17">
         <f>mtl_newcases!C31</f>
-        <v>6201</v>
+        <v>6193</v>
       </c>
       <c r="C30" s="17">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D30">
         <v>162</v>
@@ -14299,11 +14343,11 @@
       </c>
       <c r="B31" s="17">
         <f>mtl_newcases!C32</f>
-        <v>6629</v>
+        <v>6615</v>
       </c>
       <c r="C31" s="17">
         <f t="shared" si="0"/>
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -14470,11 +14514,11 @@
       </c>
       <c r="B32" s="17">
         <f>mtl_newcases!C33</f>
-        <v>7031</v>
+        <v>7010</v>
       </c>
       <c r="C32" s="17">
         <f t="shared" si="0"/>
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="D32">
         <v>242</v>
@@ -14641,7 +14685,7 @@
       </c>
       <c r="B33" s="17">
         <f>mtl_newcases!C34</f>
-        <v>7626</v>
+        <v>7605</v>
       </c>
       <c r="C33" s="17">
         <f t="shared" si="0"/>
@@ -14812,11 +14856,11 @@
       </c>
       <c r="B34" s="17">
         <f>mtl_newcases!C35</f>
-        <v>8018</v>
+        <v>7991</v>
       </c>
       <c r="C34" s="17">
         <f t="shared" si="0"/>
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D34">
         <v>391</v>
@@ -14983,11 +15027,11 @@
       </c>
       <c r="B35" s="17">
         <f>mtl_newcases!C36</f>
-        <v>8558</v>
+        <v>8526</v>
       </c>
       <c r="C35" s="17">
         <f t="shared" si="0"/>
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="D35">
         <v>454</v>
@@ -15154,11 +15198,11 @@
       </c>
       <c r="B36" s="17">
         <f>mtl_newcases!C37</f>
-        <v>8866</v>
+        <v>8830</v>
       </c>
       <c r="C36" s="17">
         <f t="shared" si="0"/>
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D36">
         <v>513</v>
@@ -15325,11 +15369,11 @@
       </c>
       <c r="B37" s="17">
         <f>mtl_newcases!C38</f>
-        <v>9248</v>
+        <v>9208</v>
       </c>
       <c r="C37" s="17">
         <f t="shared" si="0"/>
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D37">
         <v>525</v>
@@ -15465,11 +15509,11 @@
       </c>
       <c r="B38" s="17">
         <f>mtl_newcases!C39</f>
-        <v>9701</v>
+        <v>9672</v>
       </c>
       <c r="C38" s="17">
         <f t="shared" si="0"/>
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="D38">
         <v>583</v>
@@ -15636,11 +15680,11 @@
       </c>
       <c r="B39" s="17">
         <f>mtl_newcases!C40</f>
-        <v>10120</v>
+        <v>10083</v>
       </c>
       <c r="C39" s="17">
         <f t="shared" si="0"/>
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="D39">
         <v>647</v>
@@ -15807,11 +15851,11 @@
       </c>
       <c r="B40" s="17">
         <f>mtl_newcases!C41</f>
-        <v>10637</v>
+        <v>10592</v>
       </c>
       <c r="C40" s="17">
         <f t="shared" si="0"/>
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="D40">
         <v>741</v>
@@ -15978,11 +16022,11 @@
       </c>
       <c r="B41" s="17">
         <f>mtl_newcases!C42</f>
-        <v>11140</v>
+        <v>11076</v>
       </c>
       <c r="C41" s="17">
         <f t="shared" si="0"/>
-        <v>503</v>
+        <v>484</v>
       </c>
       <c r="D41">
         <v>808</v>
@@ -16149,11 +16193,11 @@
       </c>
       <c r="B42" s="17">
         <f>mtl_newcases!C43</f>
-        <v>11626</v>
+        <v>11552</v>
       </c>
       <c r="C42" s="17">
         <f t="shared" si="0"/>
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="D42">
         <v>895</v>
@@ -16320,11 +16364,11 @@
       </c>
       <c r="B43" s="17">
         <f>mtl_newcases!C44</f>
-        <v>11900</v>
+        <v>11856</v>
       </c>
       <c r="C43" s="17">
         <f t="shared" si="0"/>
-        <v>274</v>
+        <v>304</v>
       </c>
       <c r="D43">
         <v>938</v>
@@ -16491,11 +16535,11 @@
       </c>
       <c r="B44" s="17">
         <f>mtl_newcases!C45</f>
-        <v>12183</v>
+        <v>12147</v>
       </c>
       <c r="C44" s="17">
         <f>B44-B43</f>
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="D44">
         <v>983</v>
@@ -16662,11 +16706,11 @@
       </c>
       <c r="B45" s="17">
         <f>mtl_newcases!C46</f>
-        <v>12487</v>
+        <v>12573</v>
       </c>
       <c r="C45" s="17">
         <f>B45-B44</f>
-        <v>304</v>
+        <v>426</v>
       </c>
       <c r="D45">
         <v>1039</v>
@@ -16831,12 +16875,13 @@
       <c r="A46" s="19">
         <v>43949</v>
       </c>
-      <c r="B46">
-        <v>12811</v>
+      <c r="B46" s="17">
+        <f>mtl_newcases!C47</f>
+        <v>13072</v>
       </c>
       <c r="C46" s="17">
         <f t="shared" ref="C46:C47" si="438">B46-B45</f>
-        <v>324</v>
+        <v>499</v>
       </c>
       <c r="D46">
         <v>1078</v>
@@ -16970,12 +17015,13 @@
       <c r="A47" s="19">
         <v>43950</v>
       </c>
-      <c r="B47">
-        <v>13324</v>
+      <c r="B47" s="17">
+        <f>mtl_newcases!C48</f>
+        <v>13575</v>
       </c>
       <c r="C47" s="17">
         <f t="shared" si="438"/>
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="D47">
         <v>1146</v>
@@ -17109,12 +17155,13 @@
       <c r="A48" s="19">
         <v>43951</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="17">
+        <f>mtl_newcases!C49</f>
         <v>13979</v>
       </c>
       <c r="C48" s="17">
         <f t="shared" ref="C48" si="439">B48-B47</f>
-        <v>655</v>
+        <v>404</v>
       </c>
       <c r="D48">
         <v>1245</v>
@@ -17123,125 +17170,156 @@
         <f t="shared" ref="E48" si="440">D48-D47</f>
         <v>99</v>
       </c>
-      <c r="F48" t="s">
-        <v>102</v>
-      </c>
-      <c r="G48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H48" t="s">
-        <v>102</v>
-      </c>
-      <c r="I48" t="s">
-        <v>102</v>
-      </c>
-      <c r="J48" t="s">
-        <v>102</v>
-      </c>
-      <c r="K48" t="s">
-        <v>102</v>
-      </c>
-      <c r="L48" t="s">
-        <v>102</v>
-      </c>
-      <c r="M48" t="s">
-        <v>102</v>
-      </c>
-      <c r="N48" t="s">
-        <v>102</v>
-      </c>
-      <c r="O48" t="s">
-        <v>102</v>
-      </c>
-      <c r="P48" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>102</v>
-      </c>
-      <c r="R48" t="s">
-        <v>102</v>
-      </c>
-      <c r="S48" t="s">
-        <v>102</v>
-      </c>
-      <c r="T48" t="s">
-        <v>102</v>
-      </c>
-      <c r="U48" t="s">
-        <v>102</v>
-      </c>
-      <c r="V48" t="s">
-        <v>102</v>
-      </c>
-      <c r="W48" t="s">
-        <v>102</v>
-      </c>
-      <c r="X48" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AL48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AR48" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS48" t="s">
-        <v>102</v>
+      <c r="F48" cm="1">
+        <f t="array" ref="F48:O48">TRANSPOSE(santemontreal!AG$57:AG$66)</f>
+        <v>132</v>
+      </c>
+      <c r="G48">
+        <v>120</v>
+      </c>
+      <c r="H48">
+        <v>436</v>
+      </c>
+      <c r="I48">
+        <v>1553</v>
+      </c>
+      <c r="J48">
+        <v>1773</v>
+      </c>
+      <c r="K48">
+        <v>2045</v>
+      </c>
+      <c r="L48">
+        <v>1796</v>
+      </c>
+      <c r="M48">
+        <v>1241</v>
+      </c>
+      <c r="N48">
+        <v>1300</v>
+      </c>
+      <c r="O48">
+        <v>3516</v>
+      </c>
+      <c r="P48" s="18">
+        <f>F48/(age_distribution_2016!$B$2/100000)</f>
+        <v>120.28430836522691</v>
+      </c>
+      <c r="Q48" s="18">
+        <f>G48/(age_distribution_2016!$B$3/100000)</f>
+        <v>114.95904583991954</v>
+      </c>
+      <c r="R48" s="18">
+        <f>H48/(age_distribution_2016!$B$4/100000)</f>
+        <v>231.68690384462099</v>
+      </c>
+      <c r="S48" s="18">
+        <f>I48/(age_distribution_2016!$B$5/100000)</f>
+        <v>529.62741921732459</v>
+      </c>
+      <c r="T48" s="18">
+        <f>J48/(age_distribution_2016!$B$6/100000)</f>
+        <v>591.64094435638606</v>
+      </c>
+      <c r="U48" s="18">
+        <f>K48/(age_distribution_2016!$B$7/100000)</f>
+        <v>803.615286373907</v>
+      </c>
+      <c r="V48" s="18">
+        <f>L48/(age_distribution_2016!$B$8/100000)</f>
+        <v>693.77112506035724</v>
+      </c>
+      <c r="W48" s="18">
+        <f>M48/(age_distribution_2016!$B$9/100000)</f>
+        <v>605.35108899782927</v>
+      </c>
+      <c r="X48" s="18">
+        <f>N48/(age_distribution_2016!$B$10/100000)</f>
+        <v>1002.4676125848242</v>
+      </c>
+      <c r="Y48" s="18">
+        <f>O48/(age_distribution_2016!$B$11/100000)</f>
+        <v>3558.5243661758009</v>
+      </c>
+      <c r="Z48" s="3">
+        <f t="shared" ref="Z48" si="441">F48*100/SUM($F48:$O48)</f>
+        <v>0.94882116158711904</v>
+      </c>
+      <c r="AA48" s="3">
+        <f t="shared" ref="AA48" si="442">G48*100/SUM($F48:$O48)</f>
+        <v>0.86256469235192634</v>
+      </c>
+      <c r="AB48" s="3">
+        <f t="shared" ref="AB48" si="443">H48*100/SUM($F48:$O48)</f>
+        <v>3.133985048878666</v>
+      </c>
+      <c r="AC48" s="3">
+        <f t="shared" ref="AC48" si="444">I48*100/SUM($F48:$O48)</f>
+        <v>11.163024726854514</v>
+      </c>
+      <c r="AD48" s="3">
+        <f t="shared" ref="AD48" si="445">J48*100/SUM($F48:$O48)</f>
+        <v>12.744393329499712</v>
+      </c>
+      <c r="AE48" s="3">
+        <f t="shared" ref="AE48" si="446">K48*100/SUM($F48:$O48)</f>
+        <v>14.699539965497411</v>
+      </c>
+      <c r="AF48" s="3">
+        <f t="shared" ref="AF48" si="447">L48*100/SUM($F48:$O48)</f>
+        <v>12.909718228867165</v>
+      </c>
+      <c r="AG48" s="3">
+        <f t="shared" ref="AG48" si="448">M48*100/SUM($F48:$O48)</f>
+        <v>8.9203565267395053</v>
+      </c>
+      <c r="AH48" s="3">
+        <f t="shared" ref="AH48" si="449">N48*100/SUM($F48:$O48)</f>
+        <v>9.3444508338125356</v>
+      </c>
+      <c r="AI48" s="3">
+        <f t="shared" ref="AI48" si="450">O48*100/SUM($F48:$O48)</f>
+        <v>25.273145485911442</v>
+      </c>
+      <c r="AJ48" s="3">
+        <f t="shared" ref="AJ48" si="451">P48*100/SUM($P48:$Y48)</f>
+        <v>1.4576509501255785</v>
+      </c>
+      <c r="AK48" s="3">
+        <f t="shared" ref="AK48" si="452">Q48*100/SUM($P48:$Y48)</f>
+        <v>1.3931173955399463</v>
+      </c>
+      <c r="AL48" s="3">
+        <f t="shared" ref="AL48" si="453">R48*100/SUM($P48:$Y48)</f>
+        <v>2.8076699289430902</v>
+      </c>
+      <c r="AM48" s="3">
+        <f t="shared" ref="AM48" si="454">S48*100/SUM($P48:$Y48)</f>
+        <v>6.4182262950756837</v>
+      </c>
+      <c r="AN48" s="3">
+        <f t="shared" ref="AN48" si="455">T48*100/SUM($P48:$Y48)</f>
+        <v>7.1697297544057248</v>
+      </c>
+      <c r="AO48" s="3">
+        <f t="shared" ref="AO48" si="456">U48*100/SUM($P48:$Y48)</f>
+        <v>9.7385153694494946</v>
+      </c>
+      <c r="AP48" s="3">
+        <f t="shared" ref="AP48" si="457">V48*100/SUM($P48:$Y48)</f>
+        <v>8.4073820879721008</v>
+      </c>
+      <c r="AQ48" s="3">
+        <f t="shared" ref="AQ48" si="458">W48*100/SUM($P48:$Y48)</f>
+        <v>7.3358744962641413</v>
+      </c>
+      <c r="AR48" s="3">
+        <f t="shared" ref="AR48" si="459">X48*100/SUM($P48:$Y48)</f>
+        <v>12.14828341131172</v>
+      </c>
+      <c r="AS48" s="3">
+        <f t="shared" ref="AS48" si="460">Y48*100/SUM($P48:$Y48)</f>
+        <v>43.123550310912528</v>
       </c>
     </row>
   </sheetData>
@@ -17254,7 +17332,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
@@ -17278,16 +17356,16 @@
         <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E1" t="s">
         <v>164</v>
       </c>
       <c r="F1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G1" t="s">
         <v>166</v>
@@ -17299,7 +17377,7 @@
         <v>168</v>
       </c>
       <c r="J1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K1" t="s">
         <v>165</v>
@@ -19551,11 +19629,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6959A7-678F-4782-AEA8-33A89ACBBFD9}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19696,11 +19774,11 @@
         <v>43913</v>
       </c>
       <c r="B11">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -19708,11 +19786,11 @@
         <v>43914</v>
       </c>
       <c r="B12">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -19720,11 +19798,11 @@
         <v>43915</v>
       </c>
       <c r="B13">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -19736,7 +19814,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>953</v>
+        <v>949</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -19744,11 +19822,11 @@
         <v>43917</v>
       </c>
       <c r="B15">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>1197</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -19756,11 +19834,11 @@
         <v>43918</v>
       </c>
       <c r="B16">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -19768,11 +19846,11 @@
         <v>43919</v>
       </c>
       <c r="B17">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>1652</v>
+        <v>1649</v>
       </c>
       <c r="E17" s="19">
         <v>43919</v>
@@ -19782,7 +19860,7 @@
       </c>
       <c r="G17">
         <f t="shared" ref="G17:G20" si="1">C17-F17</f>
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -19790,7 +19868,7 @@
         <v>43920</v>
       </c>
       <c r="B18">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -19834,11 +19912,11 @@
         <v>43922</v>
       </c>
       <c r="B20">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>2560</v>
+        <v>2561</v>
       </c>
       <c r="E20" s="19">
         <v>43922</v>
@@ -19848,7 +19926,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>-82</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -19856,11 +19934,11 @@
         <v>43923</v>
       </c>
       <c r="B21">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>2956</v>
+        <v>2952</v>
       </c>
       <c r="E21" s="19">
         <v>43923</v>
@@ -19870,7 +19948,7 @@
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G26" si="2">C21-F21</f>
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -19878,11 +19956,11 @@
         <v>43924</v>
       </c>
       <c r="B22">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>3303</v>
+        <v>3298</v>
       </c>
       <c r="E22" s="19">
         <v>43924</v>
@@ -19892,7 +19970,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -19900,11 +19978,11 @@
         <v>43925</v>
       </c>
       <c r="B23">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>3643</v>
+        <v>3639</v>
       </c>
       <c r="E23" s="19">
         <v>43925</v>
@@ -19914,7 +19992,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>-70</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -19922,11 +20000,11 @@
         <v>43926</v>
       </c>
       <c r="B24">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>3892</v>
+        <v>3890</v>
       </c>
       <c r="E24" s="19">
         <v>43926</v>
@@ -19936,7 +20014,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>-85</v>
+        <v>-87</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -19948,7 +20026,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>4331</v>
+        <v>4329</v>
       </c>
       <c r="E25" s="19">
         <v>43927</v>
@@ -19958,7 +20036,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>-76</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -19966,11 +20044,11 @@
         <v>43928</v>
       </c>
       <c r="B26">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>4733</v>
+        <v>4732</v>
       </c>
       <c r="E26" s="19">
         <v>43928</v>
@@ -19980,7 +20058,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>-42</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -19988,11 +20066,11 @@
         <v>43929</v>
       </c>
       <c r="B27">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>5082</v>
+        <v>5080</v>
       </c>
       <c r="E27" s="19">
         <v>43929</v>
@@ -20002,7 +20080,7 @@
       </c>
       <c r="G27">
         <f t="shared" ref="G27" si="3">C27-F27</f>
-        <v>-180</v>
+        <v>-182</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -20010,11 +20088,11 @@
         <v>43930</v>
       </c>
       <c r="B28">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C28">
         <f t="shared" ref="C28:C37" si="4">C27+B28</f>
-        <v>5406</v>
+        <v>5402</v>
       </c>
       <c r="E28" s="19">
         <v>43930</v>
@@ -20024,7 +20102,7 @@
       </c>
       <c r="G28">
         <f t="shared" ref="G28:G33" si="5">C28-F28</f>
-        <v>-211</v>
+        <v>-215</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -20032,11 +20110,11 @@
         <v>43931</v>
       </c>
       <c r="B29">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C29">
         <f t="shared" si="4"/>
-        <v>5685</v>
+        <v>5680</v>
       </c>
       <c r="E29" s="19">
         <v>43931</v>
@@ -20046,7 +20124,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
-        <v>-176</v>
+        <v>-181</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -20058,7 +20136,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="4"/>
-        <v>5901</v>
+        <v>5896</v>
       </c>
       <c r="E30" s="19">
         <v>43932</v>
@@ -20068,7 +20146,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="5"/>
-        <v>-187</v>
+        <v>-192</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -20076,11 +20154,11 @@
         <v>43933</v>
       </c>
       <c r="B31">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C31">
         <f t="shared" si="4"/>
-        <v>6201</v>
+        <v>6193</v>
       </c>
       <c r="E31" s="19">
         <v>43933</v>
@@ -20090,7 +20168,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="5"/>
-        <v>-192</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -20098,11 +20176,11 @@
         <v>43934</v>
       </c>
       <c r="B32">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C32">
         <f t="shared" si="4"/>
-        <v>6629</v>
+        <v>6615</v>
       </c>
       <c r="E32" s="19">
         <v>43934</v>
@@ -20112,7 +20190,7 @@
       </c>
       <c r="G32">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -20120,11 +20198,11 @@
         <v>43935</v>
       </c>
       <c r="B33">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C33">
         <f t="shared" si="4"/>
-        <v>7031</v>
+        <v>7010</v>
       </c>
       <c r="E33" s="19">
         <v>43935</v>
@@ -20134,7 +20212,7 @@
       </c>
       <c r="G33">
         <f t="shared" si="5"/>
-        <v>201</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -20146,7 +20224,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="4"/>
-        <v>7626</v>
+        <v>7605</v>
       </c>
       <c r="E34" s="19">
         <v>43936</v>
@@ -20156,7 +20234,7 @@
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G36" si="6">C34-F34</f>
-        <v>345</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -20164,11 +20242,11 @@
         <v>43937</v>
       </c>
       <c r="B35">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C35">
         <f t="shared" si="4"/>
-        <v>8018</v>
+        <v>7991</v>
       </c>
       <c r="E35" s="19">
         <v>43937</v>
@@ -20178,7 +20256,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="6"/>
-        <v>258</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -20186,11 +20264,11 @@
         <v>43938</v>
       </c>
       <c r="B36">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="C36">
         <f t="shared" si="4"/>
-        <v>8558</v>
+        <v>8526</v>
       </c>
       <c r="E36" s="19">
         <v>43938</v>
@@ -20200,7 +20278,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="6"/>
-        <v>506</v>
+        <v>474</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -20208,11 +20286,11 @@
         <v>43939</v>
       </c>
       <c r="B37" s="23">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C37">
         <f t="shared" si="4"/>
-        <v>8866</v>
+        <v>8830</v>
       </c>
       <c r="E37" s="19">
         <v>43939</v>
@@ -20222,7 +20300,7 @@
       </c>
       <c r="G37">
         <f t="shared" ref="G37" si="7">C37-F37</f>
-        <v>409</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -20230,11 +20308,11 @@
         <v>43940</v>
       </c>
       <c r="B38" s="23">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C39" si="8">C37+B38</f>
-        <v>9248</v>
+        <v>9208</v>
       </c>
       <c r="E38" s="19">
         <v>43940</v>
@@ -20244,7 +20322,7 @@
       </c>
       <c r="G38">
         <f t="shared" ref="G38" si="9">C38-F38</f>
-        <v>284</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -20252,11 +20330,11 @@
         <v>43941</v>
       </c>
       <c r="B39">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="C39">
         <f t="shared" si="8"/>
-        <v>9701</v>
+        <v>9672</v>
       </c>
       <c r="E39" s="19">
         <v>43941</v>
@@ -20266,7 +20344,7 @@
       </c>
       <c r="G39">
         <f t="shared" ref="G39" si="10">C39-F39</f>
-        <v>353</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -20274,11 +20352,11 @@
         <v>43942</v>
       </c>
       <c r="B40">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C40">
         <f t="shared" ref="C40" si="11">C39+B40</f>
-        <v>10120</v>
+        <v>10083</v>
       </c>
       <c r="E40" s="19">
         <v>43942</v>
@@ -20288,7 +20366,7 @@
       </c>
       <c r="G40">
         <f t="shared" ref="G40" si="12">C40-F40</f>
-        <v>264</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -20296,11 +20374,11 @@
         <v>43943</v>
       </c>
       <c r="B41">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:C46" si="13">C40+B41</f>
-        <v>10637</v>
+        <f t="shared" ref="C41:C49" si="13">C40+B41</f>
+        <v>10592</v>
       </c>
       <c r="E41" s="19">
         <v>43943</v>
@@ -20310,7 +20388,7 @@
       </c>
       <c r="G41">
         <f t="shared" ref="G41" si="14">C41-F41</f>
-        <v>262</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -20318,11 +20396,11 @@
         <v>43944</v>
       </c>
       <c r="B42" s="23">
-        <v>503</v>
+        <v>484</v>
       </c>
       <c r="C42">
         <f t="shared" si="13"/>
-        <v>11140</v>
+        <v>11076</v>
       </c>
       <c r="E42" s="19">
         <v>43944</v>
@@ -20332,7 +20410,7 @@
       </c>
       <c r="G42">
         <f t="shared" ref="G42:G44" si="15">C42-F42</f>
-        <v>243</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -20340,11 +20418,11 @@
         <v>43945</v>
       </c>
       <c r="B43" s="23">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="C43">
         <f t="shared" si="13"/>
-        <v>11626</v>
+        <v>11552</v>
       </c>
       <c r="E43" s="19">
         <v>43945</v>
@@ -20354,7 +20432,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="15"/>
-        <v>465</v>
+        <v>391</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -20362,11 +20440,11 @@
         <v>43946</v>
       </c>
       <c r="B44" s="23">
-        <v>274</v>
+        <v>304</v>
       </c>
       <c r="C44">
         <f t="shared" si="13"/>
-        <v>11900</v>
+        <v>11856</v>
       </c>
       <c r="E44" s="19">
         <v>43946</v>
@@ -20376,7 +20454,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="15"/>
-        <v>279</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -20384,11 +20462,11 @@
         <v>43947</v>
       </c>
       <c r="B45" s="23">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C45">
         <f t="shared" si="13"/>
-        <v>12183</v>
+        <v>12147</v>
       </c>
       <c r="E45" s="19">
         <v>43947</v>
@@ -20398,19 +20476,19 @@
       </c>
       <c r="G45">
         <f>C45-F45</f>
-        <v>149</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="19">
         <v>43948</v>
       </c>
-      <c r="B46" s="24">
-        <v>304</v>
+      <c r="B46" s="23">
+        <v>426</v>
       </c>
       <c r="C46">
         <f t="shared" si="13"/>
-        <v>12487</v>
+        <v>12573</v>
       </c>
       <c r="E46" s="19">
         <v>43948</v>
@@ -20420,6 +20498,72 @@
       </c>
       <c r="G46">
         <f>C46-F46</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="19">
+        <v>43949</v>
+      </c>
+      <c r="B47" s="23">
+        <v>499</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="13"/>
+        <v>13072</v>
+      </c>
+      <c r="E47" s="19">
+        <v>43949</v>
+      </c>
+      <c r="F47">
+        <v>12811</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47:G49" si="16">C47-F47</f>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="19">
+        <v>43950</v>
+      </c>
+      <c r="B48" s="23">
+        <v>503</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="13"/>
+        <v>13575</v>
+      </c>
+      <c r="E48" s="19">
+        <v>43950</v>
+      </c>
+      <c r="F48">
+        <v>13324</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="16"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="19">
+        <v>43951</v>
+      </c>
+      <c r="B49" s="23">
+        <v>404</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="13"/>
+        <v>13979</v>
+      </c>
+      <c r="E49" s="19">
+        <v>43951</v>
+      </c>
+      <c r="F49">
+        <v>13979</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -20433,9 +20577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E261AEA-18EA-4FE9-ACAC-1FB61BEBD535}">
   <dimension ref="A1:HH81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG71" sqref="AG71"/>
+      <selection pane="topRight" activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20529,22 +20673,22 @@
         <v>279</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AC1" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="AF1" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="AD1" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>314</v>
-      </c>
       <c r="AG1" s="5" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="AH1" s="5"/>
       <c r="AI1" s="5"/>
@@ -20827,8 +20971,8 @@
       <c r="AF2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG2" s="7" t="s">
-        <v>102</v>
+      <c r="AG2" s="7">
+        <v>1185</v>
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="7"/>
@@ -21111,8 +21255,8 @@
       <c r="AF3" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG3" s="9" t="s">
-        <v>102</v>
+      <c r="AG3" s="9">
+        <v>324</v>
       </c>
       <c r="AH3" s="9"/>
       <c r="AI3" s="9"/>
@@ -21395,8 +21539,8 @@
       <c r="AF4" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG4" s="7" t="s">
-        <v>102</v>
+      <c r="AG4" s="7">
+        <v>6</v>
       </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
@@ -21679,8 +21823,8 @@
       <c r="AF5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG5" s="9" t="s">
-        <v>102</v>
+      <c r="AG5" s="9">
+        <v>27</v>
       </c>
       <c r="AH5" s="9"/>
       <c r="AI5" s="9"/>
@@ -21963,8 +22107,8 @@
       <c r="AF6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG6" s="7" t="s">
-        <v>102</v>
+      <c r="AG6" s="7">
+        <v>1225</v>
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
@@ -22247,8 +22391,8 @@
       <c r="AF7" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG7" s="9" t="s">
-        <v>102</v>
+      <c r="AG7" s="9">
+        <v>354</v>
       </c>
       <c r="AH7" s="9"/>
       <c r="AI7" s="9"/>
@@ -22531,8 +22675,8 @@
       <c r="AF8" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG8" s="7" t="s">
-        <v>102</v>
+      <c r="AG8" s="7">
+        <v>184</v>
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="7"/>
@@ -22815,8 +22959,8 @@
       <c r="AF9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG9" s="9" t="s">
-        <v>102</v>
+      <c r="AG9" s="9">
+        <v>95</v>
       </c>
       <c r="AH9" s="9"/>
       <c r="AI9" s="9"/>
@@ -23099,8 +23243,8 @@
       <c r="AF10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG10" s="7" t="s">
-        <v>102</v>
+      <c r="AG10" s="7">
+        <v>38</v>
       </c>
       <c r="AH10" s="7"/>
       <c r="AI10" s="7"/>
@@ -23383,8 +23527,8 @@
       <c r="AF11" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG11" s="9" t="s">
-        <v>102</v>
+      <c r="AG11" s="9">
+        <v>52</v>
       </c>
       <c r="AH11" s="9"/>
       <c r="AI11" s="9"/>
@@ -23667,8 +23811,8 @@
       <c r="AF12" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG12" s="7" t="s">
-        <v>102</v>
+      <c r="AG12" s="7">
+        <v>186</v>
       </c>
       <c r="AH12" s="7"/>
       <c r="AI12" s="7"/>
@@ -23951,8 +24095,8 @@
       <c r="AF13" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG13" s="9" t="s">
-        <v>102</v>
+      <c r="AG13" s="9">
+        <v>561</v>
       </c>
       <c r="AH13" s="9"/>
       <c r="AI13" s="9"/>
@@ -24235,8 +24379,8 @@
       <c r="AF14" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG14" s="7" t="s">
-        <v>102</v>
+      <c r="AG14" s="7">
+        <v>76</v>
       </c>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
@@ -24519,8 +24663,8 @@
       <c r="AF15" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG15" s="9" t="s">
-        <v>102</v>
+      <c r="AG15" s="9">
+        <v>1014</v>
       </c>
       <c r="AH15" s="9"/>
       <c r="AI15" s="9"/>
@@ -24803,8 +24947,8 @@
       <c r="AF16" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG16" s="7" t="s">
-        <v>102</v>
+      <c r="AG16" s="7">
+        <v>18</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="7"/>
@@ -25087,8 +25231,8 @@
       <c r="AF17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG17" s="9" t="s">
-        <v>102</v>
+      <c r="AG17" s="9">
+        <v>1316</v>
       </c>
       <c r="AH17" s="9"/>
       <c r="AI17" s="9"/>
@@ -25371,8 +25515,8 @@
       <c r="AF18" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG18" s="7" t="s">
-        <v>102</v>
+      <c r="AG18" s="7">
+        <v>11</v>
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
@@ -25655,8 +25799,8 @@
       <c r="AF19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG19" s="9" t="s">
-        <v>102</v>
+      <c r="AG19" s="9">
+        <v>125</v>
       </c>
       <c r="AH19" s="9"/>
       <c r="AI19" s="9"/>
@@ -25939,8 +26083,8 @@
       <c r="AF20" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG20" s="7" t="s">
-        <v>102</v>
+      <c r="AG20" s="7">
+        <v>194</v>
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
@@ -26223,8 +26367,8 @@
       <c r="AF21" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG21" s="9" t="s">
-        <v>102</v>
+      <c r="AG21" s="9">
+        <v>192</v>
       </c>
       <c r="AH21" s="9"/>
       <c r="AI21" s="9"/>
@@ -26507,8 +26651,8 @@
       <c r="AF22" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG22" s="7" t="s">
-        <v>102</v>
+      <c r="AG22" s="7">
+        <v>566</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="7"/>
@@ -26791,8 +26935,8 @@
       <c r="AF23" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG23" s="9" t="s">
-        <v>102</v>
+      <c r="AG23" s="9">
+        <v>83</v>
       </c>
       <c r="AH23" s="9"/>
       <c r="AI23" s="9"/>
@@ -27075,8 +27219,8 @@
       <c r="AF24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG24" s="7" t="s">
-        <v>102</v>
+      <c r="AG24" s="7">
+        <v>1029</v>
       </c>
       <c r="AH24" s="7"/>
       <c r="AI24" s="7"/>
@@ -27359,8 +27503,8 @@
       <c r="AF25" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG25" s="9" t="s">
-        <v>102</v>
+      <c r="AG25" s="9">
+        <v>777</v>
       </c>
       <c r="AH25" s="9"/>
       <c r="AI25" s="9"/>
@@ -27643,8 +27787,8 @@
       <c r="AF26" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG26" s="7" t="s">
-        <v>102</v>
+      <c r="AG26" s="7">
+        <v>10</v>
       </c>
       <c r="AH26" s="7"/>
       <c r="AI26" s="7"/>
@@ -27927,8 +28071,8 @@
       <c r="AF27" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG27" s="9" t="s">
-        <v>102</v>
+      <c r="AG27" s="9">
+        <v>518</v>
       </c>
       <c r="AH27" s="9"/>
       <c r="AI27" s="9"/>
@@ -28211,8 +28355,8 @@
       <c r="AF28" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG28" s="7" t="s">
-        <v>102</v>
+      <c r="AG28" s="7">
+        <v>582</v>
       </c>
       <c r="AH28" s="7"/>
       <c r="AI28" s="7"/>
@@ -28495,8 +28639,8 @@
       <c r="AF29" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG29" s="9" t="s">
-        <v>102</v>
+      <c r="AG29" s="20">
+        <v>2</v>
       </c>
       <c r="AH29" s="22"/>
       <c r="AI29" s="22"/>
@@ -28779,8 +28923,8 @@
       <c r="AF30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG30" s="7" t="s">
-        <v>102</v>
+      <c r="AG30" s="7">
+        <v>563</v>
       </c>
       <c r="AH30" s="7"/>
       <c r="AI30" s="7"/>
@@ -29063,8 +29207,8 @@
       <c r="AF31" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG31" s="9" t="s">
-        <v>102</v>
+      <c r="AG31" s="9">
+        <v>620</v>
       </c>
       <c r="AH31" s="9"/>
       <c r="AI31" s="9"/>
@@ -29347,8 +29491,8 @@
       <c r="AF32" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG32" s="7" t="s">
-        <v>102</v>
+      <c r="AG32" s="7">
+        <v>353</v>
       </c>
       <c r="AH32" s="7"/>
       <c r="AI32" s="7"/>
@@ -29631,8 +29775,8 @@
       <c r="AF33" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG33" s="9" t="s">
-        <v>102</v>
+      <c r="AG33" s="9">
+        <v>998</v>
       </c>
       <c r="AH33" s="9"/>
       <c r="AI33" s="9"/>
@@ -29915,8 +30059,8 @@
       <c r="AF34" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG34" s="7" t="s">
-        <v>102</v>
+      <c r="AG34" s="7">
+        <v>113</v>
       </c>
       <c r="AH34" s="7"/>
       <c r="AI34" s="7"/>
@@ -30199,8 +30343,8 @@
       <c r="AF35" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG35" s="9" t="s">
-        <v>102</v>
+      <c r="AG35" s="9">
+        <v>583</v>
       </c>
       <c r="AH35" s="9"/>
       <c r="AI35" s="9"/>
@@ -34688,22 +34832,22 @@
         <v>279</v>
       </c>
       <c r="AB56" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AC56" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD56" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE56" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="AF56" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="AD56" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="AE56" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="AF56" s="5" t="s">
-        <v>314</v>
-      </c>
       <c r="AG56" s="5" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="AH56" s="5"/>
       <c r="AI56" s="5"/>
@@ -34984,8 +35128,8 @@
       <c r="AF57" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG57" s="7" t="s">
-        <v>102</v>
+      <c r="AG57" s="7">
+        <v>132</v>
       </c>
       <c r="AH57" s="7"/>
       <c r="AI57" s="7"/>
@@ -35266,8 +35410,8 @@
       <c r="AF58" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG58" s="9" t="s">
-        <v>102</v>
+      <c r="AG58" s="9">
+        <v>120</v>
       </c>
       <c r="AH58" s="9"/>
       <c r="AI58" s="9"/>
@@ -35548,8 +35692,8 @@
       <c r="AF59" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG59" s="7" t="s">
-        <v>102</v>
+      <c r="AG59" s="7">
+        <v>436</v>
       </c>
       <c r="AH59" s="7"/>
       <c r="AI59" s="7"/>
@@ -35830,8 +35974,8 @@
       <c r="AF60" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG60" s="9" t="s">
-        <v>102</v>
+      <c r="AG60" s="9">
+        <v>1553</v>
       </c>
       <c r="AH60" s="9"/>
       <c r="AI60" s="9"/>
@@ -36112,8 +36256,8 @@
       <c r="AF61" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG61" s="7" t="s">
-        <v>102</v>
+      <c r="AG61" s="7">
+        <v>1773</v>
       </c>
       <c r="AH61" s="7"/>
       <c r="AI61" s="7"/>
@@ -36394,8 +36538,8 @@
       <c r="AF62" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG62" s="9" t="s">
-        <v>102</v>
+      <c r="AG62" s="9">
+        <v>2045</v>
       </c>
       <c r="AH62" s="9"/>
       <c r="AI62" s="9"/>
@@ -36676,8 +36820,8 @@
       <c r="AF63" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG63" s="7" t="s">
-        <v>102</v>
+      <c r="AG63" s="7">
+        <v>1796</v>
       </c>
       <c r="AH63" s="7"/>
       <c r="AI63" s="7"/>
@@ -36958,8 +37102,8 @@
       <c r="AF64" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG64" s="9" t="s">
-        <v>102</v>
+      <c r="AG64" s="9">
+        <v>1241</v>
       </c>
       <c r="AH64" s="9"/>
       <c r="AI64" s="9"/>
@@ -37240,8 +37384,8 @@
       <c r="AF65" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG65" s="7" t="s">
-        <v>102</v>
+      <c r="AG65" s="7">
+        <v>1300</v>
       </c>
       <c r="AH65" s="7"/>
       <c r="AI65" s="7"/>
@@ -37522,8 +37666,8 @@
       <c r="AF66" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AG66" s="9" t="s">
-        <v>102</v>
+      <c r="AG66" s="9">
+        <v>3516</v>
       </c>
       <c r="AH66" s="9"/>
       <c r="AI66" s="9"/>
@@ -37804,8 +37948,8 @@
       <c r="AF67" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AG67" s="7" t="s">
-        <v>102</v>
+      <c r="AG67" s="7">
+        <v>67</v>
       </c>
       <c r="AH67" s="7"/>
       <c r="AI67" s="7"/>
@@ -38086,8 +38230,8 @@
       <c r="AF68" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="AG68" s="15" t="s">
-        <v>102</v>
+      <c r="AG68" s="15">
+        <v>13979</v>
       </c>
       <c r="AH68" s="15"/>
       <c r="AI68" s="15"/>
@@ -38388,204 +38532,238 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655ECF0F-EC0D-4FC9-B182-78DF99BFDAD7}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B4:B15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D1" t="s">
-        <v>296</v>
+    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
       <c r="D3" t="s">
         <v>298</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4">
+        <v>436</v>
+      </c>
+      <c r="C4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5">
+        <v>1553</v>
+      </c>
+      <c r="C5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6">
+        <v>1773</v>
+      </c>
+      <c r="C6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" t="s">
+        <v>294</v>
+      </c>
+      <c r="F6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>2045</v>
+      </c>
+      <c r="C7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8">
+        <v>1796</v>
+      </c>
+      <c r="C8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E8">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1241</v>
+      </c>
+      <c r="C9" t="s">
+        <v>311</v>
+      </c>
+      <c r="D9" t="s">
+        <v>312</v>
+      </c>
+      <c r="E9">
         <v>87</v>
       </c>
-      <c r="B4">
-        <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D4" t="s">
-        <v>299</v>
+      <c r="F9" t="s">
+        <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5">
-        <v>109</v>
-      </c>
-      <c r="C5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" t="s">
-        <v>300</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>1300</v>
+      </c>
+      <c r="C10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" t="s">
+        <v>315</v>
+      </c>
+      <c r="E10">
+        <v>203</v>
+      </c>
+      <c r="F10" t="s">
+        <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6">
-        <v>407</v>
-      </c>
-      <c r="C6" t="s">
-        <v>289</v>
-      </c>
-      <c r="D6" t="s">
-        <v>301</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11">
+        <v>3516</v>
+      </c>
+      <c r="C11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11">
+        <v>918</v>
+      </c>
+      <c r="F11" t="s">
+        <v>319</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7">
-        <v>1412</v>
-      </c>
-      <c r="C7" t="s">
-        <v>302</v>
-      </c>
-      <c r="D7" t="s">
-        <v>303</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8">
-        <v>1629</v>
-      </c>
-      <c r="C8" t="s">
-        <v>304</v>
-      </c>
-      <c r="D8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1880</v>
-      </c>
-      <c r="C9" t="s">
-        <v>306</v>
-      </c>
-      <c r="D9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10">
-        <v>1629</v>
-      </c>
-      <c r="C10" t="s">
-        <v>304</v>
-      </c>
-      <c r="D10" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11">
-        <v>1113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>290</v>
-      </c>
-      <c r="D11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12">
-        <v>1130</v>
-      </c>
-      <c r="C12" t="s">
-        <v>280</v>
-      </c>
-      <c r="D12" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B13">
-        <v>2997</v>
+        <v>13979</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>230</v>
       </c>
       <c r="D13" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14">
-        <v>66</v>
-      </c>
-      <c r="C14" t="s">
-        <v>230</v>
-      </c>
-      <c r="D14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15">
-        <v>12486</v>
-      </c>
-      <c r="C15" t="s">
-        <v>230</v>
-      </c>
-      <c r="D15" t="s">
-        <v>292</v>
+        <v>295</v>
+      </c>
+      <c r="E13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F13" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>